<commit_message>
Remove duplicate reference to codelists for thermalProductType
</commit_message>
<xml_diff>
--- a/implementation/IMKL3_Codelists.xlsx
+++ b/implementation/IMKL3_Codelists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vlaamseoverheid.sharepoint.com/sites/informatie_vlaanderen/KLIP/Gedeelde  documenten/IMKL-PMKL/IMKL OSLO Traject 2023 + implementatiemodel/Implementatie IMKL3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\Belgif\implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{75E58E71-F091-4DC4-9F27-5EDE3D56C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA636C40-9761-4615-95CA-3CA3617DD7B1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF55A32B-CF1A-4006-9541-E8D1C70AA0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="34560" windowHeight="22452" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="624">
   <si>
     <t>nilReason</t>
   </si>
@@ -2382,37 +2382,37 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="AA1" s="11"/>
       <c r="AB1" s="11"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>526</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>451</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>277</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>346</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>455</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>286</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>458</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>322</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>417</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>192</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>489</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>399</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>409</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>339</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>508</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>405</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>435</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>494</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>518</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>444</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>335</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>468</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>329</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>426</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>17</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>555</v>
       </c>
@@ -3083,20 +3083,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64294C56-C363-4325-A21C-BEAD7C56353B}">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>605</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>599</v>
       </c>
@@ -3125,7 +3123,7 @@
         <v>ActivityValue</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>578</v>
       </c>
@@ -3140,7 +3138,7 @@
         <v>AnnotationTypeValue</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>585</v>
       </c>
@@ -3155,7 +3153,7 @@
         <v>ElectricityAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>585</v>
       </c>
@@ -3170,7 +3168,7 @@
         <v>ElectricityAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>585</v>
       </c>
@@ -3185,7 +3183,7 @@
         <v>OilGasChemicalsAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>585</v>
       </c>
@@ -3200,7 +3198,7 @@
         <v>OilGasChemicalsAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>585</v>
       </c>
@@ -3215,7 +3213,7 @@
         <v>SewerAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>585</v>
       </c>
@@ -3230,7 +3228,7 @@
         <v>SewerAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>585</v>
       </c>
@@ -3245,7 +3243,7 @@
         <v>TelecommunicationsAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>585</v>
       </c>
@@ -3260,7 +3258,7 @@
         <v>TelecommunicationsAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>585</v>
       </c>
@@ -3275,7 +3273,7 @@
         <v>ThermalAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>585</v>
       </c>
@@ -3290,7 +3288,7 @@
         <v>WaterAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>585</v>
       </c>
@@ -3305,7 +3303,7 @@
         <v>WaterAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>585</v>
       </c>
@@ -3320,7 +3318,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>585</v>
       </c>
@@ -3335,7 +3333,7 @@
         <v>ElectricitySubthemeValue</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>585</v>
       </c>
@@ -3350,7 +3348,7 @@
         <v>OilGasChemicalsSubthemeValue</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>585</v>
       </c>
@@ -3365,7 +3363,7 @@
         <v>SewerSubthemeValue</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>585</v>
       </c>
@@ -3380,7 +3378,7 @@
         <v>TelecommunicationsSubthemeValue</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>585</v>
       </c>
@@ -3395,7 +3393,7 @@
         <v>ThermalSubthemeValue</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>585</v>
       </c>
@@ -3410,7 +3408,7 @@
         <v>WaterSubthemeValue</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>585</v>
       </c>
@@ -3425,7 +3423,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>585</v>
       </c>
@@ -3440,7 +3438,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>614</v>
       </c>
@@ -3455,7 +3453,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>614</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>614</v>
       </c>
@@ -3485,7 +3483,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>602</v>
       </c>
@@ -3500,7 +3498,7 @@
         <v>ElectricityAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>602</v>
       </c>
@@ -3515,7 +3513,7 @@
         <v>ElectricityAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>602</v>
       </c>
@@ -3530,7 +3528,7 @@
         <v>OilGasChemicalsAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>602</v>
       </c>
@@ -3545,7 +3543,7 @@
         <v>OilGasChemicalsAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>602</v>
       </c>
@@ -3560,7 +3558,7 @@
         <v>SewerAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>602</v>
       </c>
@@ -3575,7 +3573,7 @@
         <v>SewerAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>602</v>
       </c>
@@ -3590,7 +3588,7 @@
         <v>TelecommunicationsAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>602</v>
       </c>
@@ -3605,7 +3603,7 @@
         <v>TelecommunicationsAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>602</v>
       </c>
@@ -3620,7 +3618,7 @@
         <v>ThermalAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>602</v>
       </c>
@@ -3635,7 +3633,7 @@
         <v>WaterAppurtenanceTypeExtendedValue</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>602</v>
       </c>
@@ -3650,7 +3648,7 @@
         <v>WaterAppurtenanceTypeIMKLValue</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>602</v>
       </c>
@@ -3665,7 +3663,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>602</v>
       </c>
@@ -3680,7 +3678,7 @@
         <v>ElectricitySubthemeValue</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>602</v>
       </c>
@@ -3695,7 +3693,7 @@
         <v>OilGasChemicalsSubthemeValue</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>602</v>
       </c>
@@ -3710,7 +3708,7 @@
         <v>SewerSubthemeValue</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>602</v>
       </c>
@@ -3725,7 +3723,7 @@
         <v>TelecommunicationsSubthemeValue</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>602</v>
       </c>
@@ -3740,7 +3738,7 @@
         <v>ThermalSubthemeValue</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>602</v>
       </c>
@@ -3755,7 +3753,7 @@
         <v>WaterSubthemeValue</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>602</v>
       </c>
@@ -3770,7 +3768,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>602</v>
       </c>
@@ -3785,7 +3783,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>580</v>
       </c>
@@ -3800,7 +3798,7 @@
         <v>DocumentMediaTypeValue</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>580</v>
       </c>
@@ -3815,7 +3813,7 @@
         <v>DocumentTypeValue</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>610</v>
       </c>
@@ -3830,7 +3828,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>610</v>
       </c>
@@ -3845,7 +3843,7 @@
         <v>ContainerTypeValue</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>610</v>
       </c>
@@ -3860,7 +3858,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>610</v>
       </c>
@@ -3875,7 +3873,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>610</v>
       </c>
@@ -3890,7 +3888,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>610</v>
       </c>
@@ -3905,7 +3903,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>610</v>
       </c>
@@ -3920,7 +3918,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>610</v>
       </c>
@@ -3935,7 +3933,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>610</v>
       </c>
@@ -3950,7 +3948,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>569</v>
       </c>
@@ -3965,7 +3963,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>569</v>
       </c>
@@ -3980,7 +3978,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>569</v>
       </c>
@@ -3995,7 +3993,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>569</v>
       </c>
@@ -4010,7 +4008,7 @@
         <v>ElectricitySubthemeValue</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>569</v>
       </c>
@@ -4025,7 +4023,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>569</v>
       </c>
@@ -4040,7 +4038,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>569</v>
       </c>
@@ -4055,7 +4053,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>569</v>
       </c>
@@ -4070,7 +4068,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>569</v>
       </c>
@@ -4085,7 +4083,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>617</v>
       </c>
@@ -4100,7 +4098,7 @@
         <v>DocumentMediaTypeValue</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>617</v>
       </c>
@@ -4115,7 +4113,7 @@
         <v>DocumentTypeValue</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>613</v>
       </c>
@@ -4130,7 +4128,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>613</v>
       </c>
@@ -4145,7 +4143,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>613</v>
       </c>
@@ -4160,7 +4158,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>572</v>
       </c>
@@ -4175,7 +4173,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>572</v>
       </c>
@@ -4190,7 +4188,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>572</v>
       </c>
@@ -4205,7 +4203,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>572</v>
       </c>
@@ -4220,7 +4218,7 @@
         <v>OilGasChemicalsProductTypeIMKLValue</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>572</v>
       </c>
@@ -4235,7 +4233,7 @@
         <v>OilGasChemicalsSubthemeValue</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>572</v>
       </c>
@@ -4250,7 +4248,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>572</v>
       </c>
@@ -4265,7 +4263,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>572</v>
       </c>
@@ -4280,7 +4278,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>572</v>
       </c>
@@ -4295,7 +4293,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>572</v>
       </c>
@@ -4310,7 +4308,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>609</v>
       </c>
@@ -4325,7 +4323,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>609</v>
       </c>
@@ -4340,7 +4338,7 @@
         <v>ContainerTypeValue</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>609</v>
       </c>
@@ -4355,7 +4353,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>609</v>
       </c>
@@ -4370,7 +4368,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>609</v>
       </c>
@@ -4385,7 +4383,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>609</v>
       </c>
@@ -4400,7 +4398,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>609</v>
       </c>
@@ -4415,7 +4413,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>609</v>
       </c>
@@ -4430,7 +4428,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>609</v>
       </c>
@@ -4445,7 +4443,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>612</v>
       </c>
@@ -4460,7 +4458,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>612</v>
       </c>
@@ -4475,7 +4473,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>612</v>
       </c>
@@ -4490,7 +4488,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>576</v>
       </c>
@@ -4505,7 +4503,7 @@
         <v>ProtectedAreaTypeValue</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>604</v>
       </c>
@@ -4520,7 +4518,7 @@
         <v>ReferenceSurfaceTypeValue</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>574</v>
       </c>
@@ -4535,7 +4533,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>574</v>
       </c>
@@ -4550,7 +4548,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>574</v>
       </c>
@@ -4565,7 +4563,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>574</v>
       </c>
@@ -4580,7 +4578,7 @@
         <v>SewerWaterTypeExtendedValue</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>574</v>
       </c>
@@ -4595,7 +4593,7 @@
         <v>SewerSubthemeValue</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>574</v>
       </c>
@@ -4610,7 +4608,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>574</v>
       </c>
@@ -4625,7 +4623,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>574</v>
       </c>
@@ -4640,7 +4638,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>574</v>
       </c>
@@ -4655,7 +4653,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>574</v>
       </c>
@@ -4670,7 +4668,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>618</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>ElectricitySubthemeValue</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>618</v>
       </c>
@@ -4700,7 +4698,7 @@
         <v>OilGasChemicalsSubthemeValue</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>618</v>
       </c>
@@ -4715,7 +4713,7 @@
         <v>SewerSubthemeValue</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>618</v>
       </c>
@@ -4730,7 +4728,7 @@
         <v>TelecommunicationsSubthemeValue</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>618</v>
       </c>
@@ -4745,7 +4743,7 @@
         <v>ThermalSubthemeValue</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>618</v>
       </c>
@@ -4760,7 +4758,7 @@
         <v>WaterSubthemeValue</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>616</v>
       </c>
@@ -4775,7 +4773,7 @@
         <v>SurveyMethodValue</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>571</v>
       </c>
@@ -4790,7 +4788,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>571</v>
       </c>
@@ -4805,7 +4803,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>571</v>
       </c>
@@ -4820,7 +4818,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>571</v>
       </c>
@@ -4835,7 +4833,7 @@
         <v>TelecommunicationsSubthemeValue</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>571</v>
       </c>
@@ -4850,7 +4848,7 @@
         <v>TelecommunicationsCableMaterialTypeExtendedValue</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>571</v>
       </c>
@@ -4865,7 +4863,7 @@
         <v>UtilityDeliveryTypeExtendedValue</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>571</v>
       </c>
@@ -4880,7 +4878,7 @@
         <v>VerticalPositionValue</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>571</v>
       </c>
@@ -4895,7 +4893,7 @@
         <v>VisibilityTypeValue</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>571</v>
       </c>
@@ -4910,7 +4908,7 @@
         <v>WarningTypeExtendedValue</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>571</v>
       </c>
@@ -4925,7 +4923,7 @@
         <v>WarningTypeIMKLValue</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>575</v>
       </c>
@@ -4940,7 +4938,7 @@
         <v>ConstructionTechniqueValue</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>575</v>
       </c>
@@ -4955,7 +4953,7 @@
         <v>ConditionOfFacilityValue</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>575</v>
       </c>
@@ -4970,7 +4968,7 @@
         <v>MaterialTypeValue</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>575</v>
       </c>
@@ -4985,7 +4983,7 @@
         <v>ThermalSubthemeValue</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>575</v>
       </c>
@@ -5000,7 +4998,7 @@
         <v>ThermalProductTypeExtendedValue</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>575</v>
       </c>
@@ -5008,355 +5006,325 @@
         <v>589</v>
       </c>
       <c r="C128" t="s">
-        <v>508</v>
+        <v>405</v>
       </c>
       <c r="D128" t="str">
         <f>VLOOKUP(C128,Overview!B:B,1,0)</f>
-        <v>ThermalProductTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+        <v>ThermalProductTypeIMKLValue</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>575</v>
       </c>
       <c r="B129" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="C129" t="s">
-        <v>405</v>
+        <v>435</v>
       </c>
       <c r="D129" t="str">
         <f>VLOOKUP(C129,Overview!B:B,1,0)</f>
-        <v>ThermalProductTypeIMKLValue</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+        <v>UtilityDeliveryTypeExtendedValue</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>575</v>
       </c>
       <c r="B130" t="s">
-        <v>589</v>
+        <v>598</v>
       </c>
       <c r="C130" t="s">
-        <v>405</v>
+        <v>518</v>
       </c>
       <c r="D130" t="str">
         <f>VLOOKUP(C130,Overview!B:B,1,0)</f>
-        <v>ThermalProductTypeIMKLValue</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VerticalPositionValue</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>575</v>
       </c>
       <c r="B131" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="C131" t="s">
-        <v>435</v>
+        <v>13</v>
       </c>
       <c r="D131" t="str">
         <f>VLOOKUP(C131,Overview!B:B,1,0)</f>
-        <v>UtilityDeliveryTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VisibilityTypeValue</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>575</v>
       </c>
       <c r="B132" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="C132" t="s">
-        <v>518</v>
+        <v>444</v>
       </c>
       <c r="D132" t="str">
         <f>VLOOKUP(C132,Overview!B:B,1,0)</f>
-        <v>VerticalPositionValue</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+        <v>WarningTypeExtendedValue</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>575</v>
       </c>
       <c r="B133" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="C133" t="s">
-        <v>13</v>
+        <v>335</v>
       </c>
       <c r="D133" t="str">
         <f>VLOOKUP(C133,Overview!B:B,1,0)</f>
-        <v>VisibilityTypeValue</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+        <v>WarningTypeIMKLValue</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="B134" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="C134" t="s">
-        <v>444</v>
+        <v>8</v>
       </c>
       <c r="D134" t="str">
         <f>VLOOKUP(C134,Overview!B:B,1,0)</f>
-        <v>WarningTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+        <v>ConditionOfFacilityValue</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="B135" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="C135" t="s">
-        <v>335</v>
+        <v>518</v>
       </c>
       <c r="D135" t="str">
         <f>VLOOKUP(C135,Overview!B:B,1,0)</f>
-        <v>WarningTypeIMKLValue</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VerticalPositionValue</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>611</v>
       </c>
       <c r="B136" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C136" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D136" t="str">
         <f>VLOOKUP(C136,Overview!B:B,1,0)</f>
-        <v>ConditionOfFacilityValue</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VisibilityTypeValue</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
       <c r="B137" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C137" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="D137" t="str">
         <f>VLOOKUP(C137,Overview!B:B,1,0)</f>
-        <v>VerticalPositionValue</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+        <v>UtilityNetworkTypeExtendedValue</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
       <c r="B138" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C138" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D138" t="str">
         <f>VLOOKUP(C138,Overview!B:B,1,0)</f>
-        <v>VisibilityTypeValue</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>ConditionOfFacilityValue</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B139" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="C139" t="s">
-        <v>494</v>
+        <v>518</v>
       </c>
       <c r="D139" t="str">
         <f>VLOOKUP(C139,Overview!B:B,1,0)</f>
-        <v>UtilityNetworkTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VerticalPositionValue</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>596</v>
+        <v>573</v>
       </c>
       <c r="B140" t="s">
-        <v>597</v>
+        <v>615</v>
       </c>
       <c r="C140" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="D140" t="str">
         <f>VLOOKUP(C140,Overview!B:B,1,0)</f>
-        <v>ConditionOfFacilityValue</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+        <v>ConstructionTechniqueValue</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>596</v>
+        <v>573</v>
       </c>
       <c r="B141" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C141" t="s">
-        <v>518</v>
+        <v>8</v>
       </c>
       <c r="D141" t="str">
         <f>VLOOKUP(C141,Overview!B:B,1,0)</f>
-        <v>VerticalPositionValue</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+        <v>ConditionOfFacilityValue</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>573</v>
       </c>
       <c r="B142" t="s">
-        <v>615</v>
+        <v>588</v>
       </c>
       <c r="C142" t="s">
-        <v>555</v>
+        <v>346</v>
       </c>
       <c r="D142" t="str">
         <f>VLOOKUP(C142,Overview!B:B,1,0)</f>
-        <v>ConstructionTechniqueValue</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>MaterialTypeValue</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>573</v>
       </c>
       <c r="B143" t="s">
-        <v>597</v>
+        <v>570</v>
       </c>
       <c r="C143" t="s">
-        <v>8</v>
+        <v>532</v>
       </c>
       <c r="D143" t="str">
         <f>VLOOKUP(C143,Overview!B:B,1,0)</f>
-        <v>ConditionOfFacilityValue</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>WaterSubthemeValue</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>573</v>
       </c>
       <c r="B144" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="C144" t="s">
-        <v>346</v>
+        <v>435</v>
       </c>
       <c r="D144" t="str">
         <f>VLOOKUP(C144,Overview!B:B,1,0)</f>
-        <v>MaterialTypeValue</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+        <v>UtilityDeliveryTypeExtendedValue</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>573</v>
       </c>
       <c r="B145" t="s">
-        <v>570</v>
+        <v>598</v>
       </c>
       <c r="C145" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="D145" t="str">
         <f>VLOOKUP(C145,Overview!B:B,1,0)</f>
-        <v>WaterSubthemeValue</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VerticalPositionValue</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>573</v>
       </c>
       <c r="B146" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="C146" t="s">
-        <v>435</v>
+        <v>13</v>
       </c>
       <c r="D146" t="str">
         <f>VLOOKUP(C146,Overview!B:B,1,0)</f>
-        <v>UtilityDeliveryTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+        <v>VisibilityTypeValue</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>573</v>
       </c>
       <c r="B147" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="C147" t="s">
-        <v>518</v>
+        <v>444</v>
       </c>
       <c r="D147" t="str">
         <f>VLOOKUP(C147,Overview!B:B,1,0)</f>
-        <v>VerticalPositionValue</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+        <v>WarningTypeExtendedValue</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>573</v>
       </c>
       <c r="B148" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="C148" t="s">
-        <v>13</v>
+        <v>335</v>
       </c>
       <c r="D148" t="str">
         <f>VLOOKUP(C148,Overview!B:B,1,0)</f>
-        <v>VisibilityTypeValue</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+        <v>WarningTypeIMKLValue</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>573</v>
       </c>
       <c r="B149" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="C149" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="D149" t="str">
         <f>VLOOKUP(C149,Overview!B:B,1,0)</f>
-        <v>WarningTypeExtendedValue</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>573</v>
-      </c>
-      <c r="B150" t="s">
-        <v>587</v>
-      </c>
-      <c r="C150" t="s">
-        <v>335</v>
-      </c>
-      <c r="D150" t="str">
-        <f>VLOOKUP(C150,Overview!B:B,1,0)</f>
-        <v>WarningTypeIMKLValue</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>573</v>
-      </c>
-      <c r="B151" t="s">
-        <v>592</v>
-      </c>
-      <c r="C151" t="s">
-        <v>426</v>
-      </c>
-      <c r="D151" t="str">
-        <f>VLOOKUP(C151,Overview!B:B,1,0)</f>
         <v>WaterTypeExtendedValue</v>
       </c>
     </row>
@@ -5366,10 +5334,10 @@
       <sortCondition ref="A1:A101"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D151">
-    <sortCondition ref="A2:A151"/>
-    <sortCondition ref="B2:B151"/>
-    <sortCondition ref="C2:C151"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D149">
+    <sortCondition ref="A2:A149"/>
+    <sortCondition ref="B2:B149"/>
+    <sortCondition ref="C2:C149"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5379,22 +5347,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B144" sqref="B144"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.33203125" customWidth="1"/>
-    <col min="7" max="7" width="97.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.28515625" customWidth="1"/>
+    <col min="7" max="7" width="97.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -5414,7 +5382,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>527</v>
       </c>
@@ -5439,7 +5407,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityTransport</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5464,7 +5432,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityTransportLocal</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>527</v>
       </c>
@@ -5489,7 +5457,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityDistributionHighVoltage</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>527</v>
       </c>
@@ -5514,7 +5482,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityDistributionLowVoltage</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>527</v>
       </c>
@@ -5539,7 +5507,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityPublicLighting</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>527</v>
       </c>
@@ -5564,7 +5532,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityTrafficLights</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>527</v>
       </c>
@@ -5589,7 +5557,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityTrafficEnforcementSystems</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>527</v>
       </c>
@@ -5614,7 +5582,7 @@
         <v>http://TODO/ElectricitySubthemeValue/electricityCathodicProtection</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>530</v>
       </c>
@@ -5639,7 +5607,7 @@
         <v>http://TODO/TelecommunicationsSubthemeValue/electronicCommunication</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>530</v>
       </c>
@@ -5664,7 +5632,7 @@
         <v>http://TODO/TelecommunicationsSubthemeValue/telecommunicationDistribution</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>530</v>
       </c>
@@ -5689,7 +5657,7 @@
         <v>http://TODO/TelecommunicationsSubthemeValue/telecommunicationMainline</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>528</v>
       </c>
@@ -5714,7 +5682,7 @@
         <v>http://TODO/OilGasChemicalsSubthemeValue/naturalGasDistributionLowPressure</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>528</v>
       </c>
@@ -5739,7 +5707,7 @@
         <v>http://TODO/OilGasChemicalsSubthemeValue/naturalGasDistributionMediumPressure</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>528</v>
       </c>
@@ -5764,7 +5732,7 @@
         <v>http://TODO/OilGasChemicalsSubthemeValue/naturalGasTransport</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>528</v>
       </c>
@@ -5789,7 +5757,7 @@
         <v>http://TODO/OilGasChemicalsSubthemeValue/oilGasChemicalsTransport</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>532</v>
       </c>
@@ -5814,7 +5782,7 @@
         <v>http://TODO/WaterSubthemeValue/drinkingWaterSupply</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>532</v>
       </c>
@@ -5839,7 +5807,7 @@
         <v>http://TODO/WaterSubthemeValue/drinkingWaterDistribution</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>529</v>
       </c>
@@ -5864,7 +5832,7 @@
         <v>http://TODO/SewerSubthemeValue/sewageWasteWaterPressurePipe</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>529</v>
       </c>
@@ -5889,7 +5857,7 @@
         <v>http://TODO/SewerSubthemeValue/sewageWasteWaterGravitationalPipe</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>529</v>
       </c>
@@ -5914,7 +5882,7 @@
         <v>http://TODO/SewerSubthemeValue/waterDrainageSurfaceWaterPressurePipe</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>529</v>
       </c>
@@ -5939,7 +5907,7 @@
         <v>http://TODO/SewerSubthemeValue/waterDrainageSurfaceWaterGravitationalPipe</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>529</v>
       </c>
@@ -5964,7 +5932,7 @@
         <v>http://TODO/SewerSubthemeValue/waterDrainagePipedCanal</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>529</v>
       </c>
@@ -5989,7 +5957,7 @@
         <v>http://TODO/SewerSubthemeValue/waterDrainageArchedWaterways</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>531</v>
       </c>
@@ -6014,7 +5982,7 @@
         <v>http://TODO/ThermalSubthemeValue/heatTransport</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>531</v>
       </c>
@@ -6039,7 +6007,7 @@
         <v>http://TODO/ThermalSubthemeValue/heatDistribution</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>531</v>
       </c>
@@ -6064,7 +6032,7 @@
         <v>http://TODO/ThermalSubthemeValue/steamTransport</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>531</v>
       </c>
@@ -6089,7 +6057,7 @@
         <v>http://TODO/ThermalSubthemeValue/steamCondensate</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -6114,7 +6082,7 @@
         <v>http://TODO/ProtectedAreaTypeValue/undergroundGasStorage</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -6139,7 +6107,7 @@
         <v>http://TODO/ProtectedAreaTypeValue/drinkingWaterExtractionArea</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -6164,7 +6132,7 @@
         <v>http://TODO/ProtectedAreaTypeValue/geothermalInstallation</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -6189,7 +6157,7 @@
         <v>http://TODO/ProtectedAreaTypeValue/otherProtectedArea</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -6211,7 +6179,7 @@
         <v>http://TODO/ProtectedAreaTypeValue/infiltrationArea</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -6236,7 +6204,7 @@
         <v>http://TODO/AnnotationTypeValue/dimensioningGuideline</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -6261,7 +6229,7 @@
         <v>http://TODO/AnnotationTypeValue/dimensioningLine</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -6286,7 +6254,7 @@
         <v>http://TODO/AnnotationTypeValue/dimensioningLabel</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -6311,7 +6279,7 @@
         <v>http://TODO/AnnotationTypeValue/arrow</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -6336,7 +6304,7 @@
         <v>http://TODO/AnnotationTypeValue/annotationLine</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>168</v>
       </c>
@@ -6361,7 +6329,7 @@
         <v>http://TODO/AnnotationTypeValue/annotationLabel</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>181</v>
       </c>
@@ -6386,7 +6354,7 @@
         <v>http://TODO/DocumentTypeValue/detailedPlan</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -6411,7 +6379,7 @@
         <v>http://TODO/DocumentTypeValue/longitudinalSection</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -6436,7 +6404,7 @@
         <v>http://TODO/DocumentTypeValue/crossSection</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -6461,7 +6429,7 @@
         <v>http://TODO/DocumentTypeValue/other</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -6486,7 +6454,7 @@
         <v>http://TODO/DocumentTypeValue/directionalDrilling</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>181</v>
       </c>
@@ -6508,7 +6476,7 @@
         <v>http://TODO/DocumentTypeValue/precaution</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -6533,7 +6501,7 @@
         <v>http://TODO/DocumentMediaTypeValue/PNG</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>183</v>
       </c>
@@ -6558,7 +6526,7 @@
         <v>http://TODO/DocumentMediaTypeValue/PDF</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>183</v>
       </c>
@@ -6583,7 +6551,7 @@
         <v>http://TODO/DocumentMediaTypeValue/JPEG</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>183</v>
       </c>
@@ -6608,7 +6576,7 @@
         <v>http://TODO/DocumentMediaTypeValue/TIFF</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -6633,7 +6601,7 @@
         <v>http://TODO/ContainerTypeValue/jacketPipe</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>193</v>
       </c>
@@ -6658,7 +6626,7 @@
         <v>http://TODO/ContainerTypeValue/cableAndPipeGutter</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -6680,7 +6648,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/carbonDioxide</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -6705,7 +6673,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/naturalGas</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -6730,7 +6698,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/bioGas</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -6755,7 +6723,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/accetone</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -6780,7 +6748,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/air</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -6805,7 +6773,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/argon</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -6830,7 +6798,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/butadiene1,2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -6855,7 +6823,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/butadiene1,3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -6880,7 +6848,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/butane </v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -6905,7 +6873,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/carbonMonoxide </v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -6930,7 +6898,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/chlorine </v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -6955,7 +6923,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/concrete</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -6980,7 +6948,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/crude</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -7005,7 +6973,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/dichloroethane </v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -7030,7 +6998,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/diesel</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -7055,7 +7023,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/ethylene </v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -7080,7 +7048,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/gasFabricationOfCocs</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -7105,7 +7073,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/gasHFx</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -7130,7 +7098,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/gasoil</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -7155,7 +7123,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/hydrogen</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -7180,7 +7148,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/isobutane </v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -7205,7 +7173,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/JET-A1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -7230,7 +7198,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/kerosene</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -7255,7 +7223,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/liquidAmmonia</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -7280,7 +7248,7 @@
         <v xml:space="preserve">http://TODO/OilGasChemicalsProductTypeIMKLValue/liquidHydrocarbon </v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -7305,7 +7273,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/multiProduct</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -7330,7 +7298,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/MVC</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -7355,7 +7323,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/nitrogen</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -7380,7 +7348,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/oxygen</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -7405,7 +7373,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/phenol</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -7430,7 +7398,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/propane</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -7455,7 +7423,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/propylene</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -7480,7 +7448,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/saltWater</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -7505,7 +7473,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/saumur</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -7530,7 +7498,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/sand</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -7555,7 +7523,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/tetrachloroide</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -7580,7 +7548,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/unknown</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -7605,7 +7573,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/water</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -7630,7 +7598,7 @@
         <v>http://TODO/OilGasChemicalsProductTypeIMKLValue/empty</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -7655,7 +7623,7 @@
         <v>http://TODO/ElectricityAppurtenanceTypeIMKLValue/grounding</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>277</v>
       </c>
@@ -7680,7 +7648,7 @@
         <v>http://TODO/ElectricityAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>277</v>
       </c>
@@ -7705,7 +7673,7 @@
         <v>http://TODO/ElectricityAppurtenanceTypeIMKLValue/marker</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -7730,7 +7698,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/airBeacon</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>286</v>
       </c>
@@ -7755,7 +7723,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/endCap</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>286</v>
       </c>
@@ -7780,7 +7748,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>286</v>
       </c>
@@ -7805,7 +7773,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/adapter</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>286</v>
       </c>
@@ -7830,7 +7798,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/valve</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>286</v>
       </c>
@@ -7855,7 +7823,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>286</v>
       </c>
@@ -7880,7 +7848,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/stoppleFitting</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>286</v>
       </c>
@@ -7905,7 +7873,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/flange</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>286</v>
       </c>
@@ -7930,7 +7898,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/sifon</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>286</v>
       </c>
@@ -7955,7 +7923,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/blowHole</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>286</v>
       </c>
@@ -7980,7 +7948,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>286</v>
       </c>
@@ -8005,7 +7973,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionInsatllation</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>286</v>
       </c>
@@ -8030,7 +7998,7 @@
         <v>http://TODO/OilGasChemicalsAppurtenanceTypeIMKLValue/sluice</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>322</v>
       </c>
@@ -8055,7 +8023,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/treatmentSystem</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>322</v>
       </c>
@@ -8080,7 +8048,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/overflow</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>322</v>
       </c>
@@ -8105,7 +8073,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>322</v>
       </c>
@@ -8130,7 +8098,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/cathodicProtectionInsatllation</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>322</v>
       </c>
@@ -8155,7 +8123,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>322</v>
       </c>
@@ -8177,7 +8145,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/infiltrationStructure</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>322</v>
       </c>
@@ -8202,7 +8170,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/effluent</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>322</v>
       </c>
@@ -8224,7 +8192,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/inlet</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>322</v>
       </c>
@@ -8246,7 +8214,7 @@
         <v>http://TODO/SewerAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>329</v>
       </c>
@@ -8271,7 +8239,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>329</v>
       </c>
@@ -8296,7 +8264,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/cathodicProtectionInsatllation</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>329</v>
       </c>
@@ -8321,7 +8289,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/connectionValve</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>329</v>
       </c>
@@ -8346,7 +8314,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>329</v>
       </c>
@@ -8368,7 +8336,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>329</v>
       </c>
@@ -8390,7 +8358,7 @@
         <v>http://TODO/WaterAppurtenanceTypeIMKLValue/drinkingWaterExtractionPoint</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>335</v>
       </c>
@@ -8415,7 +8383,7 @@
         <v>http://TODO/WarningTypeIMKLValue/protectivePlate</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>335</v>
       </c>
@@ -8437,7 +8405,7 @@
         <v>http://TODO/WarningTypeIMKLValue/geotextile</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>339</v>
       </c>
@@ -8462,7 +8430,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/dilatationJoint</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>339</v>
       </c>
@@ -8487,7 +8455,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/adapterSingleDualPipe</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>339</v>
       </c>
@@ -8512,7 +8480,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/airBeacon</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>339</v>
       </c>
@@ -8537,7 +8505,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>339</v>
       </c>
@@ -8562,7 +8530,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/adapter</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>339</v>
       </c>
@@ -8587,7 +8555,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/valve</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>339</v>
       </c>
@@ -8612,7 +8580,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>339</v>
       </c>
@@ -8637,7 +8605,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/flange</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>339</v>
       </c>
@@ -8662,7 +8630,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/sifon</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>339</v>
       </c>
@@ -8687,7 +8655,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>339</v>
       </c>
@@ -8712,7 +8680,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/cathodicProtectionInsatllation</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>339</v>
       </c>
@@ -8737,7 +8705,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/sluice</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>339</v>
       </c>
@@ -8762,7 +8730,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>339</v>
       </c>
@@ -8787,7 +8755,7 @@
         <v>http://TODO/ThermalAppurtenanceTypeIMKLValue/condensateWell</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>346</v>
       </c>
@@ -8812,7 +8780,7 @@
         <v>http://TODO/MaterialTypeValue/ductileCastIron</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>346</v>
       </c>
@@ -8837,7 +8805,7 @@
         <v>http://TODO/MaterialTypeValue/ductileCastIronBlutop</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>346</v>
       </c>
@@ -8862,7 +8830,7 @@
         <v>http://TODO/MaterialTypeValue/glassFiberReinforcedPolyester</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>346</v>
       </c>
@@ -8887,7 +8855,7 @@
         <v>http://TODO/MaterialTypeValue/grayCastIron</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>346</v>
       </c>
@@ -8912,7 +8880,7 @@
         <v>http://TODO/MaterialTypeValue/lead</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>346</v>
       </c>
@@ -8937,7 +8905,7 @@
         <v>http://TODO/MaterialTypeValue/polyethylene</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>346</v>
       </c>
@@ -8962,7 +8930,7 @@
         <v>http://TODO/MaterialTypeValue/polyethyleneSafetyLine</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>346</v>
       </c>
@@ -8987,7 +8955,7 @@
         <v>http://TODO/MaterialTypeValue/polyethyleneHighDensity</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>346</v>
       </c>
@@ -9012,7 +8980,7 @@
         <v>http://TODO/MaterialTypeValue/polypropylene</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>346</v>
       </c>
@@ -9037,7 +9005,7 @@
         <v>http://TODO/MaterialTypeValue/polypropyleneSLA</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>346</v>
       </c>
@@ -9062,7 +9030,7 @@
         <v>http://TODO/MaterialTypeValue/pvc</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>346</v>
       </c>
@@ -9087,7 +9055,7 @@
         <v>http://TODO/MaterialTypeValue/stainlessSteel</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>346</v>
       </c>
@@ -9112,7 +9080,7 @@
         <v>http://TODO/MaterialTypeValue/sideroCement</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>346</v>
       </c>
@@ -9137,7 +9105,7 @@
         <v>http://TODO/MaterialTypeValue/steel</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>346</v>
       </c>
@@ -9162,7 +9130,7 @@
         <v>http://TODO/MaterialTypeValue/fiberCement</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>346</v>
       </c>
@@ -9187,7 +9155,7 @@
         <v>http://TODO/MaterialTypeValue/prestressedConcrete</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>346</v>
       </c>
@@ -9212,7 +9180,7 @@
         <v>http://TODO/MaterialTypeValue/other</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>346</v>
       </c>
@@ -9237,7 +9205,7 @@
         <v>http://TODO/MaterialTypeValue/unknown</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>346</v>
       </c>
@@ -9262,7 +9230,7 @@
         <v>http://TODO/MaterialTypeValue/galvanisedSteel</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>346</v>
       </c>
@@ -9287,7 +9255,7 @@
         <v>http://TODO/MaterialTypeValue/concrete</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>346</v>
       </c>
@@ -9312,7 +9280,7 @@
         <v>http://TODO/MaterialTypeValue/stoneware</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>346</v>
       </c>
@@ -9337,7 +9305,7 @@
         <v>http://TODO/MaterialTypeValue/jute</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>346</v>
       </c>
@@ -9362,7 +9330,7 @@
         <v>http://TODO/MaterialTypeValue/crossLinkPolyethylene</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>346</v>
       </c>
@@ -9387,7 +9355,7 @@
         <v>http://TODO/MaterialTypeValue/brickwork</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>346</v>
       </c>
@@ -9412,7 +9380,7 @@
         <v>http://TODO/MaterialTypeValue/sulfurConcrete</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>399</v>
       </c>
@@ -9437,7 +9405,7 @@
         <v>http://TODO/TelecommunicationsAppurtenanceTypeIMKLValue/splitter</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>399</v>
       </c>
@@ -9462,7 +9430,7 @@
         <v>http://TODO/TelecommunicationsAppurtenanceTypeIMKLValue/amplifier</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>405</v>
       </c>
@@ -9487,7 +9455,7 @@
         <v>http://TODO/ThermalProductTypeIMKLValue/condensate</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>409</v>
       </c>
@@ -9512,7 +9480,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeExtendedValue/coaxial</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>409</v>
       </c>
@@ -9537,7 +9505,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeExtendedValue/opticalFiber</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>409</v>
       </c>
@@ -9562,7 +9530,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeExtendedValue/twistedPair</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>409</v>
       </c>
@@ -9587,7 +9555,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeExtendedValue/other</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>417</v>
       </c>
@@ -9612,7 +9580,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeExtendedValue/combined</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>417</v>
       </c>
@@ -9637,7 +9605,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeExtendedValue/reclaimed</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>417</v>
       </c>
@@ -9662,7 +9630,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeExtendedValue/sanitary</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>417</v>
       </c>
@@ -9687,7 +9655,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeExtendedValue/storm</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>426</v>
       </c>
@@ -9712,7 +9680,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeExtendedValue/potable</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>426</v>
       </c>
@@ -9737,7 +9705,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeExtendedValue/raw</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>426</v>
       </c>
@@ -9762,7 +9730,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeExtendedValue/salt</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>426</v>
       </c>
@@ -9787,7 +9755,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeExtendedValue/treated</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>435</v>
       </c>
@@ -9812,7 +9780,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeExtendedValue/collection</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>435</v>
       </c>
@@ -9837,7 +9805,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeExtendedValue/distribution</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>435</v>
       </c>
@@ -9862,7 +9830,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeExtendedValue/private</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>435</v>
       </c>
@@ -9887,7 +9855,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeExtendedValue/transport</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>444</v>
       </c>
@@ -9912,7 +9880,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeExtendedValue/net</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>444</v>
       </c>
@@ -9937,7 +9905,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeExtendedValue/tape</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>444</v>
       </c>
@@ -9962,7 +9930,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeExtendedValue/concretePaving</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>451</v>
       </c>
@@ -9987,7 +9955,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeExtendedValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>451</v>
       </c>
@@ -10012,7 +9980,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeExtendedValue/streetLight</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>455</v>
       </c>
@@ -10037,7 +10005,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeExtendedValue/node</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>455</v>
       </c>
@@ -10062,7 +10030,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeExtendedValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>455</v>
       </c>
@@ -10087,7 +10055,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeExtendedValue/marker</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>458</v>
       </c>
@@ -10112,7 +10080,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/catchBasin</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>458</v>
       </c>
@@ -10137,7 +10105,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/dischargeStructure</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>458</v>
       </c>
@@ -10162,7 +10130,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/other</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>458</v>
       </c>
@@ -10187,7 +10155,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/pump</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>458</v>
       </c>
@@ -10212,7 +10180,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/tideGate</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>458</v>
       </c>
@@ -10237,7 +10205,7 @@
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeExtendedValue/node</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>468</v>
       </c>
@@ -10262,7 +10230,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/hydrant</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>468</v>
       </c>
@@ -10287,7 +10255,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/meter</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>468</v>
       </c>
@@ -10312,7 +10280,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/pump</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>468</v>
       </c>
@@ -10337,7 +10305,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/systemValve</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>468</v>
       </c>
@@ -10362,7 +10330,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/thrustProtection</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>468</v>
       </c>
@@ -10387,7 +10355,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/airRelieveValve</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>468</v>
       </c>
@@ -10412,7 +10380,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/checkValve</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>468</v>
       </c>
@@ -10437,7 +10405,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/waterExhaustPoint</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>468</v>
       </c>
@@ -10462,7 +10430,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/fountain</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>468</v>
       </c>
@@ -10487,7 +10455,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/fireHydrant</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>468</v>
       </c>
@@ -10512,7 +10480,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeExtendedValue/pressureController</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>489</v>
       </c>
@@ -10537,7 +10505,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceTypeExtendedValue/spliceClosure</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>489</v>
       </c>
@@ -10562,7 +10530,7 @@
         <v>https://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceTypeExtendedValue/termination</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>494</v>
       </c>
@@ -10587,7 +10555,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/electricity</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>494</v>
       </c>
@@ -10612,7 +10580,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/oilGasChemical</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>494</v>
       </c>
@@ -10637,7 +10605,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/sewer</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>494</v>
       </c>
@@ -10662,7 +10630,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/water</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>494</v>
       </c>
@@ -10687,7 +10655,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/thermal</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>494</v>
       </c>
@@ -10712,7 +10680,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/telecommunications</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>494</v>
       </c>
@@ -10737,7 +10705,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeExtendedValue/crossTheme</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>508</v>
       </c>
@@ -10762,7 +10730,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ThermalProductTypeExtendedValue/heatingSteam</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>508</v>
       </c>
@@ -10787,7 +10755,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ThermalProductTypeExtendedValue/heatingWater</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>508</v>
       </c>
@@ -10812,7 +10780,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ThermalProductTypeExtendedValue/coolingWater</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>8</v>
       </c>
@@ -10837,7 +10805,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>8</v>
       </c>
@@ -10862,7 +10830,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -10887,7 +10855,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -10902,7 +10870,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/underConstruction</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>518</v>
       </c>
@@ -10926,7 +10894,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>518</v>
       </c>
@@ -10950,7 +10918,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>518</v>
       </c>
@@ -10974,7 +10942,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -10992,7 +10960,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -11010,7 +10978,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -11028,7 +10996,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -11046,7 +11014,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -11064,7 +11032,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>18</v>
       </c>
@@ -11086,7 +11054,7 @@
         <v>http://TODO/SurveyMethodValue/sketch</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>18</v>
       </c>
@@ -11108,7 +11076,7 @@
         <v>http://TODO/SurveyMethodValue/measuringWheel</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>18</v>
       </c>
@@ -11130,7 +11098,7 @@
         <v>http://TODO/SurveyMethodValue/digitizedPlan</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>18</v>
       </c>
@@ -11152,7 +11120,7 @@
         <v>http://TODO/SurveyMethodValue/totalStation</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>18</v>
       </c>
@@ -11174,7 +11142,7 @@
         <v>http://TODO/SurveyMethodValue/gnss</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>18</v>
       </c>
@@ -11196,7 +11164,7 @@
         <v>http://TODO/SurveyMethodValue/terrestrial</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>18</v>
       </c>
@@ -11218,7 +11186,7 @@
         <v>http://TODO/SurveyMethodValue/triangulation</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>18</v>
       </c>
@@ -11240,7 +11208,7 @@
         <v>http://TODO/SurveyMethodValue/photogrammetry</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>18</v>
       </c>
@@ -11262,7 +11230,7 @@
         <v>http://TODO/SurveyMethodValue/lidar</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>18</v>
       </c>
@@ -11284,7 +11252,7 @@
         <v>http://TODO/SurveyMethodValue/measuringTape</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>13</v>
       </c>
@@ -11306,7 +11274,7 @@
         <v>http://TODO/VisibilityTypeValue/visibleAboveGround</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>13</v>
       </c>
@@ -11328,7 +11296,7 @@
         <v>http://TODO/VisibilityTypeValue/notVisibleAboveGround</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>17</v>
       </c>
@@ -11350,7 +11318,7 @@
         <v>http://TODO/ReferenceSurfaceTypeValue/surfaceLevel</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>555</v>
       </c>
@@ -11372,7 +11340,7 @@
         <v>http://TODO/ConstructionTechniqueValue/openTrench</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>555</v>
       </c>
@@ -11394,7 +11362,7 @@
         <v>http://TODO/ConstructionTechniqueValue/directionalDrilling</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>555</v>
       </c>
@@ -11416,7 +11384,7 @@
         <v>http://TODO/ConstructionTechniqueValue/culvert</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>555</v>
       </c>

</xml_diff>

<commit_message>
Fix issues with incorrect capitalization of property names
</commit_message>
<xml_diff>
--- a/implementation/IMKL3_Codelists.xlsx
+++ b/implementation/IMKL3_Codelists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\Belgif\implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B4E823-D5A0-4834-B20C-DEC883FECC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C522BF-EF22-4241-A1B9-5485A9759045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="23040" yWindow="0" windowWidth="23040" windowHeight="30264" activeTab="1" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="625">
   <si>
     <t>nilReason</t>
   </si>
@@ -1799,9 +1799,6 @@
     <t>documentMediaType</t>
   </si>
   <si>
-    <t>containertype</t>
-  </si>
-  <si>
     <t>oilGasChemicalsProductType</t>
   </si>
   <si>
@@ -1871,9 +1868,6 @@
     <t>Check</t>
   </si>
   <si>
-    <t>ThermalSubthemevalue</t>
-  </si>
-  <si>
     <t>protectedAreaType</t>
   </si>
   <si>
@@ -1929,6 +1923,9 @@
   </si>
   <si>
     <t>leakdetectionInstallation</t>
+  </si>
+  <si>
+    <t>containerType</t>
   </si>
 </sst>
 </file>
@@ -3091,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64294C56-C363-4325-A21C-BEAD7C56353B}">
   <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3104,7 +3101,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>567</v>
@@ -3113,15 +3110,15 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B2" t="s">
         <v>598</v>
-      </c>
-      <c r="B2" t="s">
-        <v>599</v>
       </c>
       <c r="C2" t="s">
         <v>525</v>
@@ -3148,10 +3145,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B4" t="s">
         <v>584</v>
-      </c>
-      <c r="B4" t="s">
-        <v>585</v>
       </c>
       <c r="C4" t="s">
         <v>450</v>
@@ -3163,10 +3160,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>583</v>
+      </c>
+      <c r="B5" t="s">
         <v>584</v>
-      </c>
-      <c r="B5" t="s">
-        <v>585</v>
       </c>
       <c r="C5" t="s">
         <v>277</v>
@@ -3178,10 +3175,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>583</v>
+      </c>
+      <c r="B6" t="s">
         <v>584</v>
-      </c>
-      <c r="B6" t="s">
-        <v>585</v>
       </c>
       <c r="C6" t="s">
         <v>454</v>
@@ -3193,10 +3190,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>583</v>
+      </c>
+      <c r="B7" t="s">
         <v>584</v>
-      </c>
-      <c r="B7" t="s">
-        <v>585</v>
       </c>
       <c r="C7" t="s">
         <v>286</v>
@@ -3208,10 +3205,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>583</v>
+      </c>
+      <c r="B8" t="s">
         <v>584</v>
-      </c>
-      <c r="B8" t="s">
-        <v>585</v>
       </c>
       <c r="C8" t="s">
         <v>457</v>
@@ -3223,10 +3220,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>583</v>
+      </c>
+      <c r="B9" t="s">
         <v>584</v>
-      </c>
-      <c r="B9" t="s">
-        <v>585</v>
       </c>
       <c r="C9" t="s">
         <v>321</v>
@@ -3238,10 +3235,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>583</v>
+      </c>
+      <c r="B10" t="s">
         <v>584</v>
-      </c>
-      <c r="B10" t="s">
-        <v>585</v>
       </c>
       <c r="C10" t="s">
         <v>488</v>
@@ -3253,10 +3250,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>583</v>
+      </c>
+      <c r="B11" t="s">
         <v>584</v>
-      </c>
-      <c r="B11" t="s">
-        <v>585</v>
       </c>
       <c r="C11" t="s">
         <v>398</v>
@@ -3268,10 +3265,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>583</v>
+      </c>
+      <c r="B12" t="s">
         <v>584</v>
-      </c>
-      <c r="B12" t="s">
-        <v>585</v>
       </c>
       <c r="C12" t="s">
         <v>338</v>
@@ -3283,10 +3280,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" t="s">
         <v>584</v>
-      </c>
-      <c r="B13" t="s">
-        <v>585</v>
       </c>
       <c r="C13" t="s">
         <v>467</v>
@@ -3298,10 +3295,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>583</v>
+      </c>
+      <c r="B14" t="s">
         <v>584</v>
-      </c>
-      <c r="B14" t="s">
-        <v>585</v>
       </c>
       <c r="C14" t="s">
         <v>328</v>
@@ -3313,10 +3310,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3328,7 +3325,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B16" t="s">
         <v>569</v>
@@ -3343,7 +3340,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B17" t="s">
         <v>569</v>
@@ -3358,7 +3355,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B18" t="s">
         <v>569</v>
@@ -3373,7 +3370,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B19" t="s">
         <v>569</v>
@@ -3388,7 +3385,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B20" t="s">
         <v>569</v>
@@ -3403,7 +3400,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B21" t="s">
         <v>569</v>
@@ -3418,10 +3415,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C22" t="s">
         <v>517</v>
@@ -3433,10 +3430,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B23" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -3448,10 +3445,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -3463,10 +3460,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B25" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C25" t="s">
         <v>517</v>
@@ -3478,10 +3475,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B26" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
@@ -3493,10 +3490,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B27" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C27" t="s">
         <v>450</v>
@@ -3508,10 +3505,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B28" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C28" t="s">
         <v>277</v>
@@ -3523,10 +3520,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C29" t="s">
         <v>454</v>
@@ -3538,10 +3535,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C30" t="s">
         <v>286</v>
@@ -3553,10 +3550,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B31" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C31" t="s">
         <v>457</v>
@@ -3568,10 +3565,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C32" t="s">
         <v>321</v>
@@ -3583,10 +3580,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C33" t="s">
         <v>488</v>
@@ -3598,10 +3595,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B34" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C34" t="s">
         <v>398</v>
@@ -3613,10 +3610,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B35" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C35" t="s">
         <v>338</v>
@@ -3628,10 +3625,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C36" t="s">
         <v>467</v>
@@ -3643,10 +3640,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B37" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C37" t="s">
         <v>328</v>
@@ -3658,10 +3655,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B38" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B39" t="s">
         <v>569</v>
@@ -3688,7 +3685,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B40" t="s">
         <v>569</v>
@@ -3703,7 +3700,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B41" t="s">
         <v>569</v>
@@ -3718,7 +3715,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B42" t="s">
         <v>569</v>
@@ -3733,7 +3730,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B43" t="s">
         <v>569</v>
@@ -3748,7 +3745,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B44" t="s">
         <v>569</v>
@@ -3763,10 +3760,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B45" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C45" t="s">
         <v>517</v>
@@ -3778,10 +3775,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B46" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -3823,10 +3820,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B49" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C49" t="s">
         <v>554</v>
@@ -3838,10 +3835,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B50" t="s">
-        <v>582</v>
+        <v>624</v>
       </c>
       <c r="C50" t="s">
         <v>193</v>
@@ -3853,10 +3850,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B51" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -3868,10 +3865,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B52" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C52" t="s">
         <v>345</v>
@@ -3883,10 +3880,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B53" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C53" t="s">
         <v>434</v>
@@ -3898,10 +3895,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B54" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C54" t="s">
         <v>517</v>
@@ -3913,10 +3910,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B55" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -3928,10 +3925,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B56" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C56" t="s">
         <v>443</v>
@@ -3943,10 +3940,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B57" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C57" t="s">
         <v>334</v>
@@ -3961,7 +3958,7 @@
         <v>568</v>
       </c>
       <c r="B58" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C58" t="s">
         <v>554</v>
@@ -3976,7 +3973,7 @@
         <v>568</v>
       </c>
       <c r="B59" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -3991,7 +3988,7 @@
         <v>568</v>
       </c>
       <c r="B60" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C60" t="s">
         <v>345</v>
@@ -4021,7 +4018,7 @@
         <v>568</v>
       </c>
       <c r="B62" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C62" t="s">
         <v>434</v>
@@ -4036,7 +4033,7 @@
         <v>568</v>
       </c>
       <c r="B63" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C63" t="s">
         <v>517</v>
@@ -4051,7 +4048,7 @@
         <v>568</v>
       </c>
       <c r="B64" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C64" t="s">
         <v>13</v>
@@ -4066,7 +4063,7 @@
         <v>568</v>
       </c>
       <c r="B65" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C65" t="s">
         <v>443</v>
@@ -4081,7 +4078,7 @@
         <v>568</v>
       </c>
       <c r="B66" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C66" t="s">
         <v>334</v>
@@ -4093,7 +4090,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B67" t="s">
         <v>581</v>
@@ -4108,7 +4105,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B68" t="s">
         <v>580</v>
@@ -4123,10 +4120,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B69" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -4138,10 +4135,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B70" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C70" t="s">
         <v>517</v>
@@ -4153,10 +4150,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B71" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
@@ -4171,7 +4168,7 @@
         <v>571</v>
       </c>
       <c r="B72" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C72" t="s">
         <v>554</v>
@@ -4186,7 +4183,7 @@
         <v>571</v>
       </c>
       <c r="B73" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -4201,7 +4198,7 @@
         <v>571</v>
       </c>
       <c r="B74" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C74" t="s">
         <v>345</v>
@@ -4216,7 +4213,7 @@
         <v>571</v>
       </c>
       <c r="B75" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C75" t="s">
         <v>12</v>
@@ -4246,7 +4243,7 @@
         <v>571</v>
       </c>
       <c r="B77" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C77" t="s">
         <v>434</v>
@@ -4261,7 +4258,7 @@
         <v>571</v>
       </c>
       <c r="B78" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C78" t="s">
         <v>517</v>
@@ -4276,7 +4273,7 @@
         <v>571</v>
       </c>
       <c r="B79" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -4291,7 +4288,7 @@
         <v>571</v>
       </c>
       <c r="B80" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C80" t="s">
         <v>443</v>
@@ -4306,7 +4303,7 @@
         <v>571</v>
       </c>
       <c r="B81" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C81" t="s">
         <v>334</v>
@@ -4318,10 +4315,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B82" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C82" t="s">
         <v>554</v>
@@ -4333,10 +4330,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B83" t="s">
-        <v>582</v>
+        <v>624</v>
       </c>
       <c r="C83" t="s">
         <v>193</v>
@@ -4348,10 +4345,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B84" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -4363,10 +4360,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B85" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C85" t="s">
         <v>345</v>
@@ -4378,10 +4375,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B86" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C86" t="s">
         <v>434</v>
@@ -4393,10 +4390,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B87" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C87" t="s">
         <v>517</v>
@@ -4408,10 +4405,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B88" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C88" t="s">
         <v>13</v>
@@ -4423,10 +4420,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B89" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C89" t="s">
         <v>443</v>
@@ -4438,10 +4435,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B90" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C90" t="s">
         <v>334</v>
@@ -4453,10 +4450,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B91" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -4468,10 +4465,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B92" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C92" t="s">
         <v>517</v>
@@ -4483,10 +4480,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B93" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
@@ -4501,7 +4498,7 @@
         <v>575</v>
       </c>
       <c r="B94" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C94" t="s">
         <v>150</v>
@@ -4513,7 +4510,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B95" t="s">
         <v>576</v>
@@ -4531,7 +4528,7 @@
         <v>573</v>
       </c>
       <c r="B96" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C96" t="s">
         <v>554</v>
@@ -4546,7 +4543,7 @@
         <v>573</v>
       </c>
       <c r="B97" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -4561,7 +4558,7 @@
         <v>573</v>
       </c>
       <c r="B98" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C98" t="s">
         <v>345</v>
@@ -4576,7 +4573,7 @@
         <v>573</v>
       </c>
       <c r="B99" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C99" t="s">
         <v>416</v>
@@ -4606,7 +4603,7 @@
         <v>573</v>
       </c>
       <c r="B101" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C101" t="s">
         <v>434</v>
@@ -4621,7 +4618,7 @@
         <v>573</v>
       </c>
       <c r="B102" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C102" t="s">
         <v>517</v>
@@ -4636,7 +4633,7 @@
         <v>573</v>
       </c>
       <c r="B103" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C103" t="s">
         <v>13</v>
@@ -4651,7 +4648,7 @@
         <v>573</v>
       </c>
       <c r="B104" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C104" t="s">
         <v>443</v>
@@ -4666,7 +4663,7 @@
         <v>573</v>
       </c>
       <c r="B105" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C105" t="s">
         <v>334</v>
@@ -4678,7 +4675,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B106" t="s">
         <v>569</v>
@@ -4693,7 +4690,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B107" t="s">
         <v>569</v>
@@ -4708,7 +4705,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B108" t="s">
         <v>569</v>
@@ -4723,7 +4720,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B109" t="s">
         <v>569</v>
@@ -4738,7 +4735,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B110" t="s">
         <v>569</v>
@@ -4753,7 +4750,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B111" t="s">
         <v>569</v>
@@ -4768,10 +4765,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B112" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C112" t="s">
         <v>18</v>
@@ -4786,7 +4783,7 @@
         <v>570</v>
       </c>
       <c r="B113" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C113" t="s">
         <v>554</v>
@@ -4801,7 +4798,7 @@
         <v>570</v>
       </c>
       <c r="B114" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -4816,7 +4813,7 @@
         <v>570</v>
       </c>
       <c r="B115" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C115" t="s">
         <v>345</v>
@@ -4846,7 +4843,7 @@
         <v>570</v>
       </c>
       <c r="B117" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C117" t="s">
         <v>408</v>
@@ -4861,7 +4858,7 @@
         <v>570</v>
       </c>
       <c r="B118" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C118" t="s">
         <v>434</v>
@@ -4876,7 +4873,7 @@
         <v>570</v>
       </c>
       <c r="B119" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C119" t="s">
         <v>517</v>
@@ -4891,7 +4888,7 @@
         <v>570</v>
       </c>
       <c r="B120" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C120" t="s">
         <v>13</v>
@@ -4906,7 +4903,7 @@
         <v>570</v>
       </c>
       <c r="B121" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C121" t="s">
         <v>443</v>
@@ -4921,7 +4918,7 @@
         <v>570</v>
       </c>
       <c r="B122" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C122" t="s">
         <v>334</v>
@@ -4936,7 +4933,7 @@
         <v>574</v>
       </c>
       <c r="B123" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C123" t="s">
         <v>554</v>
@@ -4951,7 +4948,7 @@
         <v>574</v>
       </c>
       <c r="B124" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -4966,7 +4963,7 @@
         <v>574</v>
       </c>
       <c r="B125" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C125" t="s">
         <v>345</v>
@@ -4984,7 +4981,7 @@
         <v>569</v>
       </c>
       <c r="C126" t="s">
-        <v>606</v>
+        <v>530</v>
       </c>
       <c r="D126" t="str">
         <f>VLOOKUP(C126,Overview!B:B,1,0)</f>
@@ -4996,7 +4993,7 @@
         <v>574</v>
       </c>
       <c r="B127" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C127" t="s">
         <v>507</v>
@@ -5011,7 +5008,7 @@
         <v>574</v>
       </c>
       <c r="B128" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C128" t="s">
         <v>404</v>
@@ -5026,7 +5023,7 @@
         <v>574</v>
       </c>
       <c r="B129" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C129" t="s">
         <v>434</v>
@@ -5041,7 +5038,7 @@
         <v>574</v>
       </c>
       <c r="B130" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C130" t="s">
         <v>517</v>
@@ -5056,7 +5053,7 @@
         <v>574</v>
       </c>
       <c r="B131" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C131" t="s">
         <v>13</v>
@@ -5071,7 +5068,7 @@
         <v>574</v>
       </c>
       <c r="B132" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C132" t="s">
         <v>443</v>
@@ -5086,7 +5083,7 @@
         <v>574</v>
       </c>
       <c r="B133" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C133" t="s">
         <v>334</v>
@@ -5098,10 +5095,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B134" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -5113,10 +5110,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B135" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C135" t="s">
         <v>517</v>
@@ -5128,10 +5125,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B136" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C136" t="s">
         <v>13</v>
@@ -5143,10 +5140,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>592</v>
+      </c>
+      <c r="B137" t="s">
         <v>593</v>
-      </c>
-      <c r="B137" t="s">
-        <v>594</v>
       </c>
       <c r="C137" t="s">
         <v>493</v>
@@ -5158,10 +5155,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>594</v>
+      </c>
+      <c r="B138" t="s">
         <v>595</v>
-      </c>
-      <c r="B138" t="s">
-        <v>596</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -5173,10 +5170,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B139" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C139" t="s">
         <v>517</v>
@@ -5191,7 +5188,7 @@
         <v>572</v>
       </c>
       <c r="B140" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C140" t="s">
         <v>554</v>
@@ -5206,7 +5203,7 @@
         <v>572</v>
       </c>
       <c r="B141" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -5221,7 +5218,7 @@
         <v>572</v>
       </c>
       <c r="B142" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C142" t="s">
         <v>345</v>
@@ -5251,7 +5248,7 @@
         <v>572</v>
       </c>
       <c r="B144" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C144" t="s">
         <v>434</v>
@@ -5266,7 +5263,7 @@
         <v>572</v>
       </c>
       <c r="B145" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C145" t="s">
         <v>517</v>
@@ -5281,7 +5278,7 @@
         <v>572</v>
       </c>
       <c r="B146" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C146" t="s">
         <v>13</v>
@@ -5296,7 +5293,7 @@
         <v>572</v>
       </c>
       <c r="B147" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C147" t="s">
         <v>443</v>
@@ -5311,7 +5308,7 @@
         <v>572</v>
       </c>
       <c r="B148" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C148" t="s">
         <v>334</v>
@@ -5326,7 +5323,7 @@
         <v>572</v>
       </c>
       <c r="B149" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C149" t="s">
         <v>425</v>
@@ -5355,9 +5352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
   <dimension ref="A1:G249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G138" sqref="G138"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6202,7 +6199,7 @@
         <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>561</v>
@@ -6227,7 +6224,7 @@
         <v>156</v>
       </c>
       <c r="E35" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>561</v>
@@ -6252,7 +6249,7 @@
         <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>561</v>
@@ -7971,7 +7968,7 @@
         <v>317</v>
       </c>
       <c r="E105" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>561</v>
@@ -8096,7 +8093,7 @@
         <v>317</v>
       </c>
       <c r="E110" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>561</v>
@@ -8262,7 +8259,7 @@
         <v>317</v>
       </c>
       <c r="E117" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F117" s="9" t="s">
         <v>561</v>
@@ -8353,10 +8350,10 @@
         <v>WaterAppurtenanceTypeIMKLValue</v>
       </c>
       <c r="C121" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F121" s="10" t="s">
         <v>533</v>
@@ -8678,7 +8675,7 @@
         <v>317</v>
       </c>
       <c r="E134" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F134" s="9" t="s">
         <v>561</v>
@@ -8772,7 +8769,7 @@
         <v>ThermalAppurtenanceTypeIMKLValue</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F138" s="10" t="s">
         <v>533</v>
@@ -8791,7 +8788,7 @@
         <v>ThermalAppurtenanceTypeIMKLValue</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F139" s="10" t="s">
         <v>533</v>
@@ -11460,15 +11457,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -11728,15 +11716,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791B434E-C5B6-43DF-B218-859297235BBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11754,4 +11743,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Replace references in examples with new URIs
</commit_message>
<xml_diff>
--- a/implementation/IMKL3_Codelists.xlsx
+++ b/implementation/IMKL3_Codelists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\IMKL 3\Implementatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3806060B-5780-426A-969F-EF72FD828151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC19ACD-40ED-402C-9BB1-0D82638EDBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -2548,7 +2548,7 @@
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5786,8 +5786,8 @@
   <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9875,7 +9875,7 @@
         <v>402</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>559</v>
+        <v>649</v>
       </c>
       <c r="G165" s="4" t="str">
         <f>VLOOKUP(A165,Overview!B:D,3,0)&amp; "/" &amp; E165</f>
@@ -10999,8 +10999,8 @@
       <c r="E210" t="s">
         <v>398</v>
       </c>
-      <c r="F210" s="5" t="s">
-        <v>199</v>
+      <c r="F210" s="8" t="s">
+        <v>649</v>
       </c>
       <c r="G210" s="4" t="str">
         <f>VLOOKUP(A210,Overview!B:D,3,0)&amp; "/" &amp; E210</f>

</xml_diff>

<commit_message>
Remove unnecessary white space
</commit_message>
<xml_diff>
--- a/implementation/IMKL3_Codelists.xlsx
+++ b/implementation/IMKL3_Codelists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\IMKL 3\Implementatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1225DFC-210E-4ED2-9F5F-D096A1EA23F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E145F50-ECA0-4E97-879C-01E7B8D7ADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Codelist Usage'!$A$1:$D$155</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Codelists!$A$1:$H$250</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Codelists!$A$1:$I$250</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$E$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="859">
   <si>
     <t>nilReason</t>
   </si>
@@ -2599,6 +2599,39 @@
 The security connections between and within distribution areas, with the aim of ensuring the supplied capacities of these distribution areas;
 The transport of drinking water between water production centres and between the water extractions and these water distribution centres;
 The transport of drinking water to large customers (port areas, a large company, an airport,...)</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>oilGasChemicals</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>liquidHydrocarbon</t>
+  </si>
+  <si>
+    <t>butane</t>
+  </si>
+  <si>
+    <t>carbonMonoxide</t>
+  </si>
+  <si>
+    <t>chlorine</t>
+  </si>
+  <si>
+    <t>dichloroethane</t>
+  </si>
+  <si>
+    <t>ethylene</t>
+  </si>
+  <si>
+    <t>isobutane</t>
   </si>
 </sst>
 </file>
@@ -3062,7 +3095,7 @@
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6298,11 +6331,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
-  <dimension ref="A1:H250"/>
+  <dimension ref="A1:I250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F181" sqref="F181"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6316,10 +6349,13 @@
     <col min="8" max="8" width="97.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>851</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>533</v>
       </c>
@@ -6338,8 +6374,11 @@
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>524</v>
       </c>
@@ -6366,8 +6405,11 @@
         <f>VLOOKUP(A2,Overview!B:D,3,0)&amp; "/" &amp; E2</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityCathodicProtection</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -6394,8 +6436,11 @@
         <f>VLOOKUP(A3,Overview!B:D,3,0)&amp; "/" &amp; E3</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityDistributionHighVoltage</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>524</v>
       </c>
@@ -6422,8 +6467,11 @@
         <f>VLOOKUP(A4,Overview!B:D,3,0)&amp; "/" &amp; E4</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityDistributionLowVoltage</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>524</v>
       </c>
@@ -6450,8 +6498,11 @@
         <f>VLOOKUP(A5,Overview!B:D,3,0)&amp; "/" &amp; E5</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityPublicLighting</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>524</v>
       </c>
@@ -6478,8 +6529,11 @@
         <f>VLOOKUP(A6,Overview!B:D,3,0)&amp; "/" &amp; E6</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityTrafficEnforcementSystems</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>524</v>
       </c>
@@ -6506,8 +6560,11 @@
         <f>VLOOKUP(A7,Overview!B:D,3,0)&amp; "/" &amp; E7</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityTrafficLights</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>524</v>
       </c>
@@ -6534,8 +6591,11 @@
         <f>VLOOKUP(A8,Overview!B:D,3,0)&amp; "/" &amp; E8</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityTransport</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>524</v>
       </c>
@@ -6562,8 +6622,11 @@
         <f>VLOOKUP(A9,Overview!B:D,3,0)&amp; "/" &amp; E9</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricitySubthemeValue/electricityTransportLocal</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>527</v>
       </c>
@@ -6590,8 +6653,11 @@
         <f>VLOOKUP(A10,Overview!B:D,3,0)&amp; "/" &amp; E10</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsSubthemeValue/electronicCommunication</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>527</v>
       </c>
@@ -6618,8 +6684,11 @@
         <f>VLOOKUP(A11,Overview!B:D,3,0)&amp; "/" &amp; E11</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsSubthemeValue/telecommunicationDistribution</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>527</v>
       </c>
@@ -6646,8 +6715,11 @@
         <f>VLOOKUP(A12,Overview!B:D,3,0)&amp; "/" &amp; E12</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsSubthemeValue/telecommunicationMainline</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>525</v>
       </c>
@@ -6674,8 +6746,11 @@
         <f>VLOOKUP(A13,Overview!B:D,3,0)&amp; "/" &amp; E13</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasDistributionLowPressure</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>525</v>
       </c>
@@ -6702,8 +6777,11 @@
         <f>VLOOKUP(A14,Overview!B:D,3,0)&amp; "/" &amp; E14</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasDistributionMediumPressure</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>525</v>
       </c>
@@ -6730,8 +6808,11 @@
         <f>VLOOKUP(A15,Overview!B:D,3,0)&amp; "/" &amp; E15</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasTransport</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>525</v>
       </c>
@@ -6758,8 +6839,11 @@
         <f>VLOOKUP(A16,Overview!B:D,3,0)&amp; "/" &amp; E16</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/oilGasChemicalsTransport</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="60">
+      <c r="I16" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60">
       <c r="A17" t="s">
         <v>529</v>
       </c>
@@ -6786,8 +6870,11 @@
         <f>VLOOKUP(A17,Overview!B:D,3,0)&amp; "/" &amp; E17</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterSubthemeValue/drinkingWaterDistribution</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="195">
+      <c r="I17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="195">
       <c r="A18" t="s">
         <v>529</v>
       </c>
@@ -6814,8 +6901,11 @@
         <f>VLOOKUP(A18,Overview!B:D,3,0)&amp; "/" &amp; E18</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterSubthemeValue/drinkingWaterSupply</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>526</v>
       </c>
@@ -6842,8 +6932,11 @@
         <f>VLOOKUP(A19,Overview!B:D,3,0)&amp; "/" &amp; E19</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/sewageWasteWaterGravitationalPipe</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>526</v>
       </c>
@@ -6870,8 +6963,11 @@
         <f>VLOOKUP(A20,Overview!B:D,3,0)&amp; "/" &amp; E20</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/sewageWasteWaterPressurePipe</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>526</v>
       </c>
@@ -6898,8 +6994,11 @@
         <f>VLOOKUP(A21,Overview!B:D,3,0)&amp; "/" &amp; E21</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/waterDrainageArchedWaterways</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>526</v>
       </c>
@@ -6926,8 +7025,11 @@
         <f>VLOOKUP(A22,Overview!B:D,3,0)&amp; "/" &amp; E22</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/waterDrainagePipedCanal</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>526</v>
       </c>
@@ -6954,8 +7056,11 @@
         <f>VLOOKUP(A23,Overview!B:D,3,0)&amp; "/" &amp; E23</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/waterDrainageSurfaceWaterGravitationalPipe</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>526</v>
       </c>
@@ -6982,8 +7087,11 @@
         <f>VLOOKUP(A24,Overview!B:D,3,0)&amp; "/" &amp; E24</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerSubthemeValue/waterDrainageSurfaceWaterPressurePipe</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>528</v>
       </c>
@@ -7010,8 +7118,11 @@
         <f>VLOOKUP(A25,Overview!B:D,3,0)&amp; "/" &amp; E25</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalSubthemeValue/heatDistribution</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>528</v>
       </c>
@@ -7038,8 +7149,11 @@
         <f>VLOOKUP(A26,Overview!B:D,3,0)&amp; "/" &amp; E26</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalSubthemeValue/heatTransport</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>528</v>
       </c>
@@ -7066,8 +7180,11 @@
         <f>VLOOKUP(A27,Overview!B:D,3,0)&amp; "/" &amp; E27</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalSubthemeValue/steamCondensate</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>528</v>
       </c>
@@ -7094,8 +7211,11 @@
         <f>VLOOKUP(A28,Overview!B:D,3,0)&amp; "/" &amp; E28</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalSubthemeValue/steamTransport</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -7122,8 +7242,11 @@
         <f>VLOOKUP(A29,Overview!B:D,3,0)&amp; "/" &amp; E29</f>
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/drinkingWaterExtractionArea</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -7150,8 +7273,11 @@
         <f>VLOOKUP(A30,Overview!B:D,3,0)&amp; "/" &amp; E30</f>
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/geothermalInstallation</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -7175,8 +7301,11 @@
         <f>VLOOKUP(A31,Overview!B:D,3,0)&amp; "/" &amp; E31</f>
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/infiltrationArea</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -7203,8 +7332,11 @@
         <f>VLOOKUP(A32,Overview!B:D,3,0)&amp; "/" &amp; E32</f>
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/otherProtectedArea</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -7231,8 +7363,11 @@
         <f>VLOOKUP(A33,Overview!B:D,3,0)&amp; "/" &amp; E33</f>
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/undergroundGasStorage</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -7259,8 +7394,11 @@
         <f>VLOOKUP(A34,Overview!B:D,3,0)&amp; "/" &amp; E34</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/annotationLabel</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>167</v>
       </c>
@@ -7287,8 +7425,11 @@
         <f>VLOOKUP(A35,Overview!B:D,3,0)&amp; "/" &amp; E35</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/annotationLine</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>167</v>
       </c>
@@ -7315,8 +7456,11 @@
         <f>VLOOKUP(A36,Overview!B:D,3,0)&amp; "/" &amp; E36</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/arrow</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -7343,8 +7487,11 @@
         <f>VLOOKUP(A37,Overview!B:D,3,0)&amp; "/" &amp; E37</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningGuideline</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -7371,8 +7518,11 @@
         <f>VLOOKUP(A38,Overview!B:D,3,0)&amp; "/" &amp; E38</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningLabel</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>167</v>
       </c>
@@ -7399,8 +7549,11 @@
         <f>VLOOKUP(A39,Overview!B:D,3,0)&amp; "/" &amp; E39</f>
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningLine</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>180</v>
       </c>
@@ -7427,8 +7580,11 @@
         <f>VLOOKUP(A40,Overview!B:D,3,0)&amp; "/" &amp; E40</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/crossSection</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -7455,8 +7611,11 @@
         <f>VLOOKUP(A41,Overview!B:D,3,0)&amp; "/" &amp; E41</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/detailedPlan</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>180</v>
       </c>
@@ -7483,8 +7642,11 @@
         <f>VLOOKUP(A42,Overview!B:D,3,0)&amp; "/" &amp; E42</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/directionalDrilling</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>180</v>
       </c>
@@ -7511,8 +7673,11 @@
         <f>VLOOKUP(A43,Overview!B:D,3,0)&amp; "/" &amp; E43</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/longitudinalSection</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -7539,8 +7704,11 @@
         <f>VLOOKUP(A44,Overview!B:D,3,0)&amp; "/" &amp; E44</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/other</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>180</v>
       </c>
@@ -7564,8 +7732,11 @@
         <f>VLOOKUP(A45,Overview!B:D,3,0)&amp; "/" &amp; E45</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/precaution</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>182</v>
       </c>
@@ -7592,8 +7763,11 @@
         <f>VLOOKUP(A46,Overview!B:D,3,0)&amp; "/" &amp; E46</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/JPEG</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>182</v>
       </c>
@@ -7620,8 +7794,11 @@
         <f>VLOOKUP(A47,Overview!B:D,3,0)&amp; "/" &amp; E47</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/PDF</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -7648,8 +7825,11 @@
         <f>VLOOKUP(A48,Overview!B:D,3,0)&amp; "/" &amp; E48</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/PNG</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>182</v>
       </c>
@@ -7676,8 +7856,11 @@
         <f>VLOOKUP(A49,Overview!B:D,3,0)&amp; "/" &amp; E49</f>
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/TIFF</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>192</v>
       </c>
@@ -7704,8 +7887,11 @@
         <f>VLOOKUP(A50,Overview!B:D,3,0)&amp; "/" &amp; E50</f>
         <v>https://vocab.belgif.be/auth/IMKL-ContainerTypeValue/cableAndPipeGutter</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>192</v>
       </c>
@@ -7732,8 +7918,11 @@
         <f>VLOOKUP(A51,Overview!B:D,3,0)&amp; "/" &amp; E51</f>
         <v>https://vocab.belgif.be/auth/IMKL-ContainerTypeValue/jacketPipe</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -7760,8 +7949,11 @@
         <f>VLOOKUP(A52,Overview!B:D,3,0)&amp; "/" &amp; E52</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/accetone</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -7788,8 +7980,11 @@
         <f>VLOOKUP(A53,Overview!B:D,3,0)&amp; "/" &amp; E53</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/air</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -7816,8 +8011,11 @@
         <f>VLOOKUP(A54,Overview!B:D,3,0)&amp; "/" &amp; E54</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/argon</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -7844,8 +8042,11 @@
         <f>VLOOKUP(A55,Overview!B:D,3,0)&amp; "/" &amp; E55</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/bioGas</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -7872,8 +8073,11 @@
         <f>VLOOKUP(A56,Overview!B:D,3,0)&amp; "/" &amp; E56</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butadiene1,2</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -7900,8 +8104,11 @@
         <f>VLOOKUP(A57,Overview!B:D,3,0)&amp; "/" &amp; E57</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butadiene1,3</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -7916,7 +8123,7 @@
         <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>216</v>
+        <v>853</v>
       </c>
       <c r="F58" t="s">
         <v>760</v>
@@ -7926,10 +8133,13 @@
       </c>
       <c r="H58" s="4" t="str">
         <f>VLOOKUP(A58,Overview!B:D,3,0)&amp; "/" &amp; E58</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butane </v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butane</v>
+      </c>
+      <c r="I58" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -7953,8 +8163,11 @@
         <f>VLOOKUP(A59,Overview!B:D,3,0)&amp; "/" &amp; E59</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/carbonDioxide</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -7969,7 +8182,7 @@
         <v>219</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
+        <v>854</v>
       </c>
       <c r="F60" t="s">
         <v>762</v>
@@ -7979,10 +8192,13 @@
       </c>
       <c r="H60" s="4" t="str">
         <f>VLOOKUP(A60,Overview!B:D,3,0)&amp; "/" &amp; E60</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/carbonMonoxide </v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/carbonMonoxide</v>
+      </c>
+      <c r="I60" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -7997,7 +8213,7 @@
         <v>221</v>
       </c>
       <c r="E61" t="s">
-        <v>220</v>
+        <v>855</v>
       </c>
       <c r="F61" t="s">
         <v>752</v>
@@ -8007,10 +8223,13 @@
       </c>
       <c r="H61" s="4" t="str">
         <f>VLOOKUP(A61,Overview!B:D,3,0)&amp; "/" &amp; E61</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/chlorine </v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/chlorine</v>
+      </c>
+      <c r="I61" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -8037,8 +8256,11 @@
         <f>VLOOKUP(A62,Overview!B:D,3,0)&amp; "/" &amp; E62</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/concrete</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -8065,8 +8287,11 @@
         <f>VLOOKUP(A63,Overview!B:D,3,0)&amp; "/" &amp; E63</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/crude</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -8081,7 +8306,7 @@
         <v>227</v>
       </c>
       <c r="E64" t="s">
-        <v>226</v>
+        <v>856</v>
       </c>
       <c r="F64" t="s">
         <v>763</v>
@@ -8091,10 +8316,13 @@
       </c>
       <c r="H64" s="4" t="str">
         <f>VLOOKUP(A64,Overview!B:D,3,0)&amp; "/" &amp; E64</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/dichloroethane </v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/dichloroethane</v>
+      </c>
+      <c r="I64" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -8121,8 +8349,11 @@
         <f>VLOOKUP(A65,Overview!B:D,3,0)&amp; "/" &amp; E65</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/diesel</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -8149,8 +8380,11 @@
         <f>VLOOKUP(A66,Overview!B:D,3,0)&amp; "/" &amp; E66</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/empty</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -8165,7 +8399,7 @@
         <v>230</v>
       </c>
       <c r="E67" t="s">
-        <v>229</v>
+        <v>857</v>
       </c>
       <c r="F67" t="s">
         <v>764</v>
@@ -8175,10 +8409,13 @@
       </c>
       <c r="H67" s="4" t="str">
         <f>VLOOKUP(A67,Overview!B:D,3,0)&amp; "/" &amp; E67</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/ethylene </v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/ethylene</v>
+      </c>
+      <c r="I67" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -8205,8 +8442,11 @@
         <f>VLOOKUP(A68,Overview!B:D,3,0)&amp; "/" &amp; E68</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasFabricationOfCocs</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -8233,8 +8473,11 @@
         <f>VLOOKUP(A69,Overview!B:D,3,0)&amp; "/" &amp; E69</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasHFx</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -8261,8 +8504,11 @@
         <f>VLOOKUP(A70,Overview!B:D,3,0)&amp; "/" &amp; E70</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasoil</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -8289,8 +8535,11 @@
         <f>VLOOKUP(A71,Overview!B:D,3,0)&amp; "/" &amp; E71</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/hydrogen</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -8305,7 +8554,7 @@
         <v>240</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
+        <v>858</v>
       </c>
       <c r="F72" t="s">
         <v>767</v>
@@ -8315,10 +8564,13 @@
       </c>
       <c r="H72" s="4" t="str">
         <f>VLOOKUP(A72,Overview!B:D,3,0)&amp; "/" &amp; E72</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/isobutane </v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/isobutane</v>
+      </c>
+      <c r="I72" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -8345,8 +8597,11 @@
         <f>VLOOKUP(A73,Overview!B:D,3,0)&amp; "/" &amp; E73</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/JET-A1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -8373,8 +8628,11 @@
         <f>VLOOKUP(A74,Overview!B:D,3,0)&amp; "/" &amp; E74</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/kerosene</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -8401,8 +8659,11 @@
         <f>VLOOKUP(A75,Overview!B:D,3,0)&amp; "/" &amp; E75</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/liquidAmmonia</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -8417,7 +8678,7 @@
         <v>248</v>
       </c>
       <c r="E76" t="s">
-        <v>247</v>
+        <v>852</v>
       </c>
       <c r="F76" s="13" t="s">
         <v>771</v>
@@ -8427,10 +8688,13 @@
       </c>
       <c r="H76" s="4" t="str">
         <f>VLOOKUP(A76,Overview!B:D,3,0)&amp; "/" &amp; E76</f>
-        <v xml:space="preserve">https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/liquidHydrocarbon </v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/liquidHydrocarbon</v>
+      </c>
+      <c r="I76" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -8457,8 +8721,11 @@
         <f>VLOOKUP(A77,Overview!B:D,3,0)&amp; "/" &amp; E77</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/multiProduct</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -8485,8 +8752,11 @@
         <f>VLOOKUP(A78,Overview!B:D,3,0)&amp; "/" &amp; E78</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/MVC</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -8513,8 +8783,11 @@
         <f>VLOOKUP(A79,Overview!B:D,3,0)&amp; "/" &amp; E79</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/naturalGas</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -8541,8 +8814,11 @@
         <f>VLOOKUP(A80,Overview!B:D,3,0)&amp; "/" &amp; E80</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/nitrogen</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -8569,8 +8845,11 @@
         <f>VLOOKUP(A81,Overview!B:D,3,0)&amp; "/" &amp; E81</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/oxygen</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -8597,8 +8876,11 @@
         <f>VLOOKUP(A82,Overview!B:D,3,0)&amp; "/" &amp; E82</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/phenol</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -8625,8 +8907,11 @@
         <f>VLOOKUP(A83,Overview!B:D,3,0)&amp; "/" &amp; E83</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/propane</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -8653,8 +8938,11 @@
         <f>VLOOKUP(A84,Overview!B:D,3,0)&amp; "/" &amp; E84</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/propylene</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -8681,8 +8969,11 @@
         <f>VLOOKUP(A85,Overview!B:D,3,0)&amp; "/" &amp; E85</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/saltWater</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -8709,8 +9000,11 @@
         <f>VLOOKUP(A86,Overview!B:D,3,0)&amp; "/" &amp; E86</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/sand</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -8737,8 +9031,11 @@
         <f>VLOOKUP(A87,Overview!B:D,3,0)&amp; "/" &amp; E87</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/saumur</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -8765,8 +9062,11 @@
         <f>VLOOKUP(A88,Overview!B:D,3,0)&amp; "/" &amp; E88</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/tetrachloroide</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -8793,8 +9093,11 @@
         <f>VLOOKUP(A89,Overview!B:D,3,0)&amp; "/" &amp; E89</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/unknown</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -8821,8 +9124,11 @@
         <f>VLOOKUP(A90,Overview!B:D,3,0)&amp; "/" &amp; E90</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/water</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>276</v>
       </c>
@@ -8849,8 +9155,11 @@
         <f>VLOOKUP(A91,Overview!B:D,3,0)&amp; "/" &amp; E91</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricityAppurtenanceTypeIMKLValue/grounding</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>276</v>
       </c>
@@ -8877,8 +9186,11 @@
         <f>VLOOKUP(A92,Overview!B:D,3,0)&amp; "/" &amp; E92</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricityAppurtenanceTypeIMKLValue/marker</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -8905,8 +9217,11 @@
         <f>VLOOKUP(A93,Overview!B:D,3,0)&amp; "/" &amp; E93</f>
         <v>https://vocab.belgif.be/auth/IMKL-ElectricityAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>285</v>
       </c>
@@ -8933,8 +9248,11 @@
         <f>VLOOKUP(A94,Overview!B:D,3,0)&amp; "/" &amp; E94</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/adapter</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>285</v>
       </c>
@@ -8961,8 +9279,11 @@
         <f>VLOOKUP(A95,Overview!B:D,3,0)&amp; "/" &amp; E95</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/airBeacon</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>285</v>
       </c>
@@ -8989,8 +9310,11 @@
         <f>VLOOKUP(A96,Overview!B:D,3,0)&amp; "/" &amp; E96</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/blowHole</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>285</v>
       </c>
@@ -9017,8 +9341,11 @@
         <f>VLOOKUP(A97,Overview!B:D,3,0)&amp; "/" &amp; E97</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionInstallation</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>285</v>
       </c>
@@ -9045,8 +9372,11 @@
         <f>VLOOKUP(A98,Overview!B:D,3,0)&amp; "/" &amp; E98</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>285</v>
       </c>
@@ -9073,8 +9403,11 @@
         <f>VLOOKUP(A99,Overview!B:D,3,0)&amp; "/" &amp; E99</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/endCap</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>285</v>
       </c>
@@ -9101,8 +9434,11 @@
         <f>VLOOKUP(A100,Overview!B:D,3,0)&amp; "/" &amp; E100</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/flange</v>
       </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="I100" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>285</v>
       </c>
@@ -9129,8 +9465,11 @@
         <f>VLOOKUP(A101,Overview!B:D,3,0)&amp; "/" &amp; E101</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>285</v>
       </c>
@@ -9157,8 +9496,11 @@
         <f>VLOOKUP(A102,Overview!B:D,3,0)&amp; "/" &amp; E102</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/siphon</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>285</v>
       </c>
@@ -9185,8 +9527,11 @@
         <f>VLOOKUP(A103,Overview!B:D,3,0)&amp; "/" &amp; E103</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="I103" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>285</v>
       </c>
@@ -9213,8 +9558,11 @@
         <f>VLOOKUP(A104,Overview!B:D,3,0)&amp; "/" &amp; E104</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/sluice</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>285</v>
       </c>
@@ -9241,8 +9589,11 @@
         <f>VLOOKUP(A105,Overview!B:D,3,0)&amp; "/" &amp; E105</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/stoppleFitting</v>
       </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>285</v>
       </c>
@@ -9269,8 +9620,11 @@
         <f>VLOOKUP(A106,Overview!B:D,3,0)&amp; "/" &amp; E106</f>
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/valve</v>
       </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>320</v>
       </c>
@@ -9297,8 +9651,11 @@
         <f>VLOOKUP(A107,Overview!B:D,3,0)&amp; "/" &amp; E107</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/cathodicProtectionInstallation</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>320</v>
       </c>
@@ -9325,8 +9682,11 @@
         <f>VLOOKUP(A108,Overview!B:D,3,0)&amp; "/" &amp; E108</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>320</v>
       </c>
@@ -9353,8 +9713,11 @@
         <f>VLOOKUP(A109,Overview!B:D,3,0)&amp; "/" &amp; E109</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>320</v>
       </c>
@@ -9381,8 +9744,11 @@
         <f>VLOOKUP(A110,Overview!B:D,3,0)&amp; "/" &amp; E110</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/effluent</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>320</v>
       </c>
@@ -9406,8 +9772,11 @@
         <f>VLOOKUP(A111,Overview!B:D,3,0)&amp; "/" &amp; E111</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/infiltrationStructure</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>320</v>
       </c>
@@ -9431,8 +9800,11 @@
         <f>VLOOKUP(A112,Overview!B:D,3,0)&amp; "/" &amp; E112</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/inlet</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>320</v>
       </c>
@@ -9456,8 +9828,11 @@
         <f>VLOOKUP(A113,Overview!B:D,3,0)&amp; "/" &amp; E113</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>320</v>
       </c>
@@ -9484,8 +9859,11 @@
         <f>VLOOKUP(A114,Overview!B:D,3,0)&amp; "/" &amp; E114</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/other</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>320</v>
       </c>
@@ -9512,8 +9890,11 @@
         <f>VLOOKUP(A115,Overview!B:D,3,0)&amp; "/" &amp; E115</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/overflow</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>327</v>
       </c>
@@ -9540,8 +9921,11 @@
         <f>VLOOKUP(A116,Overview!B:D,3,0)&amp; "/" &amp; E116</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/cathodicProtectionInstallation</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>327</v>
       </c>
@@ -9568,8 +9952,11 @@
         <f>VLOOKUP(A117,Overview!B:D,3,0)&amp; "/" &amp; E117</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="I117" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>327</v>
       </c>
@@ -9596,8 +9983,11 @@
         <f>VLOOKUP(A118,Overview!B:D,3,0)&amp; "/" &amp; E118</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/connectionValve</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="I118" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119" t="s">
         <v>327</v>
       </c>
@@ -9624,8 +10014,11 @@
         <f>VLOOKUP(A119,Overview!B:D,3,0)&amp; "/" &amp; E119</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>327</v>
       </c>
@@ -9649,8 +10042,11 @@
         <f>VLOOKUP(A120,Overview!B:D,3,0)&amp; "/" &amp; E120</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/drinkingWaterExtractionPoint</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="I120" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>327</v>
       </c>
@@ -9674,8 +10070,11 @@
         <f>VLOOKUP(A121,Overview!B:D,3,0)&amp; "/" &amp; E121</f>
         <v>https://vocab.belgif.be/auth/IMKL-WaterAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="I121" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>635</v>
       </c>
@@ -9699,8 +10098,11 @@
         <f>VLOOKUP(A122,Overview!B:D,3,0)&amp; "/" &amp; E122</f>
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/concretePaving</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>333</v>
       </c>
@@ -9724,8 +10126,11 @@
         <f>VLOOKUP(A123,Overview!B:D,3,0)&amp; "/" &amp; E123</f>
         <v>https://vocab.belgif.be/auth/IMKL-WarningTypeIMKLValue/geotextile</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="I123" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>337</v>
       </c>
@@ -9752,8 +10157,11 @@
         <f>VLOOKUP(A124,Overview!B:D,3,0)&amp; "/" &amp; E124</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/adapter</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="I124" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>337</v>
       </c>
@@ -9780,8 +10188,11 @@
         <f>VLOOKUP(A125,Overview!B:D,3,0)&amp; "/" &amp; E125</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/adapterSingleDualPipe</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>337</v>
       </c>
@@ -9808,8 +10219,11 @@
         <f>VLOOKUP(A126,Overview!B:D,3,0)&amp; "/" &amp; E126</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/airBeacon</v>
       </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="I126" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>337</v>
       </c>
@@ -9836,8 +10250,11 @@
         <f>VLOOKUP(A127,Overview!B:D,3,0)&amp; "/" &amp; E127</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/cathodicProtectionInstallation</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="I127" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>337</v>
       </c>
@@ -9864,8 +10281,11 @@
         <f>VLOOKUP(A128,Overview!B:D,3,0)&amp; "/" &amp; E128</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="I128" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>337</v>
       </c>
@@ -9892,8 +10312,11 @@
         <f>VLOOKUP(A129,Overview!B:D,3,0)&amp; "/" &amp; E129</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/condensateWell</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="I129" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>337</v>
       </c>
@@ -9920,8 +10343,11 @@
         <f>VLOOKUP(A130,Overview!B:D,3,0)&amp; "/" &amp; E130</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/deliveryPoint</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="I130" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>337</v>
       </c>
@@ -9948,8 +10374,11 @@
         <f>VLOOKUP(A131,Overview!B:D,3,0)&amp; "/" &amp; E131</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/dilatationJoint</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="I131" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>337</v>
       </c>
@@ -9976,8 +10405,11 @@
         <f>VLOOKUP(A132,Overview!B:D,3,0)&amp; "/" &amp; E132</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/flange</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="I132" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133" t="s">
         <v>337</v>
       </c>
@@ -9998,8 +10430,11 @@
         <f>VLOOKUP(A133,Overview!B:D,3,0)&amp; "/" &amp; E133</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/leakdetectionInstallation</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="I133" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>337</v>
       </c>
@@ -10020,8 +10455,11 @@
         <f>VLOOKUP(A134,Overview!B:D,3,0)&amp; "/" &amp; E134</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/leakdetectionMeasurementPoint</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="I134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>337</v>
       </c>
@@ -10048,8 +10486,11 @@
         <f>VLOOKUP(A135,Overview!B:D,3,0)&amp; "/" &amp; E135</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="I135" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>337</v>
       </c>
@@ -10076,8 +10517,11 @@
         <f>VLOOKUP(A136,Overview!B:D,3,0)&amp; "/" &amp; E136</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/siphon</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>337</v>
       </c>
@@ -10104,8 +10548,11 @@
         <f>VLOOKUP(A137,Overview!B:D,3,0)&amp; "/" &amp; E137</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="I137" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>337</v>
       </c>
@@ -10132,8 +10579,11 @@
         <f>VLOOKUP(A138,Overview!B:D,3,0)&amp; "/" &amp; E138</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/sluice</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="I138" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>337</v>
       </c>
@@ -10160,8 +10610,11 @@
         <f>VLOOKUP(A139,Overview!B:D,3,0)&amp; "/" &amp; E139</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalAppurtenanceTypeIMKLValue/valve</v>
       </c>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="I139" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>344</v>
       </c>
@@ -10188,8 +10641,11 @@
         <f>VLOOKUP(A140,Overview!B:D,3,0)&amp; "/" &amp; E140</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/brickwork</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="I140" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>344</v>
       </c>
@@ -10216,8 +10672,11 @@
         <f>VLOOKUP(A141,Overview!B:D,3,0)&amp; "/" &amp; E141</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/concrete</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="I141" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>344</v>
       </c>
@@ -10244,8 +10703,11 @@
         <f>VLOOKUP(A142,Overview!B:D,3,0)&amp; "/" &amp; E142</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/crossLinkPolyethylene</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="I142" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>344</v>
       </c>
@@ -10272,8 +10734,11 @@
         <f>VLOOKUP(A143,Overview!B:D,3,0)&amp; "/" &amp; E143</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/ductileCastIron</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="I143" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>344</v>
       </c>
@@ -10300,8 +10765,11 @@
         <f>VLOOKUP(A144,Overview!B:D,3,0)&amp; "/" &amp; E144</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/ductileCastIronBlutop</v>
       </c>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="I144" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>344</v>
       </c>
@@ -10328,8 +10796,11 @@
         <f>VLOOKUP(A145,Overview!B:D,3,0)&amp; "/" &amp; E145</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/fiberCement</v>
       </c>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="I145" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>344</v>
       </c>
@@ -10356,8 +10827,11 @@
         <f>VLOOKUP(A146,Overview!B:D,3,0)&amp; "/" &amp; E146</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/galvanisedSteel</v>
       </c>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="I146" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>344</v>
       </c>
@@ -10384,8 +10858,11 @@
         <f>VLOOKUP(A147,Overview!B:D,3,0)&amp; "/" &amp; E147</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/glassFiberReinforcedPolyester</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="I147" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
       <c r="A148" t="s">
         <v>344</v>
       </c>
@@ -10412,8 +10889,11 @@
         <f>VLOOKUP(A148,Overview!B:D,3,0)&amp; "/" &amp; E148</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/grayCastIron</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="I148" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
       <c r="A149" t="s">
         <v>344</v>
       </c>
@@ -10440,8 +10920,11 @@
         <f>VLOOKUP(A149,Overview!B:D,3,0)&amp; "/" &amp; E149</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/jute</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="I149" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
       <c r="A150" t="s">
         <v>344</v>
       </c>
@@ -10468,8 +10951,11 @@
         <f>VLOOKUP(A150,Overview!B:D,3,0)&amp; "/" &amp; E150</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/lead</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="I150" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
       <c r="A151" t="s">
         <v>344</v>
       </c>
@@ -10496,8 +10982,11 @@
         <f>VLOOKUP(A151,Overview!B:D,3,0)&amp; "/" &amp; E151</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/other</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="I151" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
       <c r="A152" t="s">
         <v>344</v>
       </c>
@@ -10524,8 +11013,11 @@
         <f>VLOOKUP(A152,Overview!B:D,3,0)&amp; "/" &amp; E152</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethylene</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="I152" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
       <c r="A153" t="s">
         <v>344</v>
       </c>
@@ -10552,8 +11044,11 @@
         <f>VLOOKUP(A153,Overview!B:D,3,0)&amp; "/" &amp; E153</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethyleneHighDensity</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="I153" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
       <c r="A154" t="s">
         <v>344</v>
       </c>
@@ -10580,8 +11075,11 @@
         <f>VLOOKUP(A154,Overview!B:D,3,0)&amp; "/" &amp; E154</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethyleneSafetyLine</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="I154" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
       <c r="A155" t="s">
         <v>344</v>
       </c>
@@ -10608,8 +11106,11 @@
         <f>VLOOKUP(A155,Overview!B:D,3,0)&amp; "/" &amp; E155</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polypropylene</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="I155" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
       <c r="A156" t="s">
         <v>344</v>
       </c>
@@ -10636,8 +11137,11 @@
         <f>VLOOKUP(A156,Overview!B:D,3,0)&amp; "/" &amp; E156</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polypropyleneSLA</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="I156" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
       <c r="A157" t="s">
         <v>344</v>
       </c>
@@ -10664,8 +11168,11 @@
         <f>VLOOKUP(A157,Overview!B:D,3,0)&amp; "/" &amp; E157</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/prestressedConcrete</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="I157" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
       <c r="A158" t="s">
         <v>344</v>
       </c>
@@ -10692,8 +11199,11 @@
         <f>VLOOKUP(A158,Overview!B:D,3,0)&amp; "/" &amp; E158</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/pvc</v>
       </c>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="I158" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
       <c r="A159" t="s">
         <v>344</v>
       </c>
@@ -10720,8 +11230,11 @@
         <f>VLOOKUP(A159,Overview!B:D,3,0)&amp; "/" &amp; E159</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/sideroCement</v>
       </c>
-    </row>
-    <row r="160" spans="1:8">
+      <c r="I159" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
       <c r="A160" t="s">
         <v>344</v>
       </c>
@@ -10748,8 +11261,11 @@
         <f>VLOOKUP(A160,Overview!B:D,3,0)&amp; "/" &amp; E160</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/stainlessSteel</v>
       </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="I160" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>344</v>
       </c>
@@ -10776,8 +11292,11 @@
         <f>VLOOKUP(A161,Overview!B:D,3,0)&amp; "/" &amp; E161</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/steel</v>
       </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="I161" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>344</v>
       </c>
@@ -10804,8 +11323,11 @@
         <f>VLOOKUP(A162,Overview!B:D,3,0)&amp; "/" &amp; E162</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/stoneware</v>
       </c>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="I162" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>344</v>
       </c>
@@ -10832,8 +11354,11 @@
         <f>VLOOKUP(A163,Overview!B:D,3,0)&amp; "/" &amp; E163</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/sulfurConcrete</v>
       </c>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="I163" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>344</v>
       </c>
@@ -10860,8 +11385,11 @@
         <f>VLOOKUP(A164,Overview!B:D,3,0)&amp; "/" &amp; E164</f>
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/unknown</v>
       </c>
-    </row>
-    <row r="165" spans="1:8">
+      <c r="I164" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>397</v>
       </c>
@@ -10888,8 +11416,11 @@
         <f>VLOOKUP(A165,Overview!B:D,3,0)&amp; "/" &amp; E165</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsAppurtenanceTypeIMKLValue/amplifier</v>
       </c>
-    </row>
-    <row r="166" spans="1:8">
+      <c r="I165" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>397</v>
       </c>
@@ -10916,8 +11447,11 @@
         <f>VLOOKUP(A166,Overview!B:D,3,0)&amp; "/" &amp; E166</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsAppurtenanceTypeIMKLValue/spliceClosure</v>
       </c>
-    </row>
-    <row r="167" spans="1:8">
+      <c r="I166" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>403</v>
       </c>
@@ -10944,8 +11478,11 @@
         <f>VLOOKUP(A167,Overview!B:D,3,0)&amp; "/" &amp; E167</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalProductTypeIMKLValue/condensate</v>
       </c>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="I167" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>651</v>
       </c>
@@ -10972,8 +11509,11 @@
         <f>VLOOKUP(A168,Overview!B:D,3,0)&amp; "/" &amp; E168</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsCableMaterialTypeIMKLValue/coaxial</v>
       </c>
-    </row>
-    <row r="169" spans="1:8">
+      <c r="I168" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>651</v>
       </c>
@@ -11000,8 +11540,11 @@
         <f>VLOOKUP(A169,Overview!B:D,3,0)&amp; "/" &amp; E169</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsCableMaterialTypeIMKLValue/opticalFiber</v>
       </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="I169" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>651</v>
       </c>
@@ -11028,8 +11571,11 @@
         <f>VLOOKUP(A170,Overview!B:D,3,0)&amp; "/" &amp; E170</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsCableMaterialTypeIMKLValue/other</v>
       </c>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="I170" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>651</v>
       </c>
@@ -11056,8 +11602,11 @@
         <f>VLOOKUP(A171,Overview!B:D,3,0)&amp; "/" &amp; E171</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsCableMaterialTypeIMKLValue/twistedPair</v>
       </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="I171" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
       <c r="A172" t="s">
         <v>639</v>
       </c>
@@ -11081,8 +11630,11 @@
         <f>VLOOKUP(A172,Overview!B:D,3,0)&amp; "/" &amp; E172</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/combined</v>
       </c>
-    </row>
-    <row r="173" spans="1:8">
+      <c r="I172" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>639</v>
       </c>
@@ -11106,8 +11658,11 @@
         <f>VLOOKUP(A173,Overview!B:D,3,0)&amp; "/" &amp; E173</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/reclaimed</v>
       </c>
-    </row>
-    <row r="174" spans="1:8">
+      <c r="I173" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>639</v>
       </c>
@@ -11131,8 +11686,11 @@
         <f>VLOOKUP(A174,Overview!B:D,3,0)&amp; "/" &amp; E174</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/sanitary</v>
       </c>
-    </row>
-    <row r="175" spans="1:8">
+      <c r="I174" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>639</v>
       </c>
@@ -11156,8 +11714,11 @@
         <f>VLOOKUP(A175,Overview!B:D,3,0)&amp; "/" &amp; E175</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/storm</v>
       </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="I175" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>637</v>
       </c>
@@ -11181,8 +11742,11 @@
         <f>VLOOKUP(A176,Overview!B:D,3,0)&amp; "/" &amp; E176</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeValue/potable</v>
       </c>
-    </row>
-    <row r="177" spans="1:8">
+      <c r="I176" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>637</v>
       </c>
@@ -11206,8 +11770,11 @@
         <f>VLOOKUP(A177,Overview!B:D,3,0)&amp; "/" &amp; E177</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeValue/raw</v>
       </c>
-    </row>
-    <row r="178" spans="1:8">
+      <c r="I177" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>637</v>
       </c>
@@ -11231,8 +11798,11 @@
         <f>VLOOKUP(A178,Overview!B:D,3,0)&amp; "/" &amp; E178</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeValue/salt</v>
       </c>
-    </row>
-    <row r="179" spans="1:8">
+      <c r="I178" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>637</v>
       </c>
@@ -11256,8 +11826,11 @@
         <f>VLOOKUP(A179,Overview!B:D,3,0)&amp; "/" &amp; E179</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterTypeValue/treated</v>
       </c>
-    </row>
-    <row r="180" spans="1:8">
+      <c r="I179" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>632</v>
       </c>
@@ -11281,8 +11854,11 @@
         <f>VLOOKUP(A180,Overview!B:D,3,0)&amp; "/" &amp; E180</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/collection</v>
       </c>
-    </row>
-    <row r="181" spans="1:8">
+      <c r="I180" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>632</v>
       </c>
@@ -11306,8 +11882,11 @@
         <f>VLOOKUP(A181,Overview!B:D,3,0)&amp; "/" &amp; E181</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/distribution</v>
       </c>
-    </row>
-    <row r="182" spans="1:8">
+      <c r="I181" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>632</v>
       </c>
@@ -11331,8 +11910,11 @@
         <f>VLOOKUP(A182,Overview!B:D,3,0)&amp; "/" &amp; E182</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/private</v>
       </c>
-    </row>
-    <row r="183" spans="1:8">
+      <c r="I182" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>632</v>
       </c>
@@ -11356,8 +11938,11 @@
         <f>VLOOKUP(A183,Overview!B:D,3,0)&amp; "/" &amp; E183</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/transport</v>
       </c>
-    </row>
-    <row r="184" spans="1:8">
+      <c r="I183" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>654</v>
       </c>
@@ -11384,8 +11969,11 @@
         <f>VLOOKUP(A184,Overview!B:D,3,0)&amp; "/" &amp; E184</f>
         <v>https://vocab.belgif.be/auth/IMKL-UtilityDeliveryTypeIMKLValue/connection</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" ht="30">
+      <c r="I184" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="30">
       <c r="A185" t="s">
         <v>635</v>
       </c>
@@ -11409,8 +11997,11 @@
         <f>VLOOKUP(A185,Overview!B:D,3,0)&amp; "/" &amp; E185</f>
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/net</v>
       </c>
-    </row>
-    <row r="186" spans="1:8">
+      <c r="I185" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
         <v>333</v>
       </c>
@@ -11437,8 +12028,11 @@
         <f>VLOOKUP(A186,Overview!B:D,3,0)&amp; "/" &amp; E186</f>
         <v>https://vocab.belgif.be/auth/IMKL-WarningTypeIMKLValue/protectivePlate</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" ht="60">
+      <c r="I186" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="60">
       <c r="A187" t="s">
         <v>635</v>
       </c>
@@ -11462,8 +12056,11 @@
         <f>VLOOKUP(A187,Overview!B:D,3,0)&amp; "/" &amp; E187</f>
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
-    </row>
-    <row r="188" spans="1:8">
+      <c r="I187" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
       <c r="A188" t="s">
         <v>625</v>
       </c>
@@ -11487,8 +12084,11 @@
         <f>VLOOKUP(A188,Overview!B:D,3,0)&amp; "/" &amp; E188</f>
         <v>https://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/deliveryPoint</v>
       </c>
-    </row>
-    <row r="189" spans="1:8">
+      <c r="I188" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9">
       <c r="A189" t="s">
         <v>625</v>
       </c>
@@ -11512,8 +12112,11 @@
         <f>VLOOKUP(A189,Overview!B:D,3,0)&amp; "/" &amp; E189</f>
         <v>https://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/streetLight</v>
       </c>
-    </row>
-    <row r="190" spans="1:8">
+      <c r="I189" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9">
       <c r="A190" t="s">
         <v>626</v>
       </c>
@@ -11537,8 +12140,11 @@
         <f>VLOOKUP(A190,Overview!B:D,3,0)&amp; "/" &amp; E190</f>
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
-    </row>
-    <row r="191" spans="1:8">
+      <c r="I190" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
       <c r="A191" t="s">
         <v>626</v>
       </c>
@@ -11562,8 +12168,11 @@
         <f>VLOOKUP(A191,Overview!B:D,3,0)&amp; "/" &amp; E191</f>
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
-    </row>
-    <row r="192" spans="1:8">
+      <c r="I191" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9">
       <c r="A192" t="s">
         <v>626</v>
       </c>
@@ -11587,8 +12196,11 @@
         <f>VLOOKUP(A192,Overview!B:D,3,0)&amp; "/" &amp; E192</f>
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
-    </row>
-    <row r="193" spans="1:8">
+      <c r="I192" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9">
       <c r="A193" t="s">
         <v>628</v>
       </c>
@@ -11612,8 +12224,11 @@
         <f>VLOOKUP(A193,Overview!B:D,3,0)&amp; "/" &amp; E193</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/catchBasin</v>
       </c>
-    </row>
-    <row r="194" spans="1:8">
+      <c r="I193" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9">
       <c r="A194" t="s">
         <v>628</v>
       </c>
@@ -11637,8 +12252,11 @@
         <f>VLOOKUP(A194,Overview!B:D,3,0)&amp; "/" &amp; E194</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/dischargeStructure</v>
       </c>
-    </row>
-    <row r="195" spans="1:8">
+      <c r="I194" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9">
       <c r="A195" t="s">
         <v>320</v>
       </c>
@@ -11665,8 +12283,11 @@
         <f>VLOOKUP(A195,Overview!B:D,3,0)&amp; "/" &amp; E195</f>
         <v>https://vocab.belgif.be/auth/IMKL-SewerAppurtenanceTypeIMKLValue/treatmentSystem</v>
       </c>
-    </row>
-    <row r="196" spans="1:8">
+      <c r="I195" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9">
       <c r="A196" t="s">
         <v>628</v>
       </c>
@@ -11690,8 +12311,11 @@
         <f>VLOOKUP(A196,Overview!B:D,3,0)&amp; "/" &amp; E196</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/pump</v>
       </c>
-    </row>
-    <row r="197" spans="1:8">
+      <c r="I196" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9">
       <c r="A197" t="s">
         <v>628</v>
       </c>
@@ -11715,8 +12339,11 @@
         <f>VLOOKUP(A197,Overview!B:D,3,0)&amp; "/" &amp; E197</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/sewerNode</v>
       </c>
-    </row>
-    <row r="198" spans="1:8">
+      <c r="I197" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9">
       <c r="A198" t="s">
         <v>628</v>
       </c>
@@ -11740,8 +12367,11 @@
         <f>VLOOKUP(A198,Overview!B:D,3,0)&amp; "/" &amp; E198</f>
         <v>https://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/tideGate</v>
       </c>
-    </row>
-    <row r="199" spans="1:8">
+      <c r="I198" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9">
       <c r="A199" t="s">
         <v>630</v>
       </c>
@@ -11765,8 +12395,11 @@
         <f>VLOOKUP(A199,Overview!B:D,3,0)&amp; "/" &amp; E199</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/airRelieveValve</v>
       </c>
-    </row>
-    <row r="200" spans="1:8">
+      <c r="I199" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9">
       <c r="A200" t="s">
         <v>630</v>
       </c>
@@ -11790,8 +12423,11 @@
         <f>VLOOKUP(A200,Overview!B:D,3,0)&amp; "/" &amp; E200</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/checkValve</v>
       </c>
-    </row>
-    <row r="201" spans="1:8">
+      <c r="I200" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9">
       <c r="A201" t="s">
         <v>630</v>
       </c>
@@ -11815,8 +12451,11 @@
         <f>VLOOKUP(A201,Overview!B:D,3,0)&amp; "/" &amp; E201</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fireHydrant</v>
       </c>
-    </row>
-    <row r="202" spans="1:8">
+      <c r="I201" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9">
       <c r="A202" t="s">
         <v>630</v>
       </c>
@@ -11840,8 +12479,11 @@
         <f>VLOOKUP(A202,Overview!B:D,3,0)&amp; "/" &amp; E202</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fountain</v>
       </c>
-    </row>
-    <row r="203" spans="1:8">
+      <c r="I202" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9">
       <c r="A203" t="s">
         <v>630</v>
       </c>
@@ -11865,8 +12507,11 @@
         <f>VLOOKUP(A203,Overview!B:D,3,0)&amp; "/" &amp; E203</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/hydrant</v>
       </c>
-    </row>
-    <row r="204" spans="1:8">
+      <c r="I203" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9">
       <c r="A204" t="s">
         <v>630</v>
       </c>
@@ -11890,8 +12535,11 @@
         <f>VLOOKUP(A204,Overview!B:D,3,0)&amp; "/" &amp; E204</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/meter</v>
       </c>
-    </row>
-    <row r="205" spans="1:8">
+      <c r="I204" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9">
       <c r="A205" t="s">
         <v>630</v>
       </c>
@@ -11915,8 +12563,11 @@
         <f>VLOOKUP(A205,Overview!B:D,3,0)&amp; "/" &amp; E205</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pressureController</v>
       </c>
-    </row>
-    <row r="206" spans="1:8">
+      <c r="I205" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9">
       <c r="A206" t="s">
         <v>630</v>
       </c>
@@ -11940,8 +12591,11 @@
         <f>VLOOKUP(A206,Overview!B:D,3,0)&amp; "/" &amp; E206</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pump</v>
       </c>
-    </row>
-    <row r="207" spans="1:8">
+      <c r="I206" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9">
       <c r="A207" t="s">
         <v>630</v>
       </c>
@@ -11965,8 +12619,11 @@
         <f>VLOOKUP(A207,Overview!B:D,3,0)&amp; "/" &amp; E207</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/systemValve</v>
       </c>
-    </row>
-    <row r="208" spans="1:8">
+      <c r="I207" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9">
       <c r="A208" t="s">
         <v>630</v>
       </c>
@@ -11990,8 +12647,11 @@
         <f>VLOOKUP(A208,Overview!B:D,3,0)&amp; "/" &amp; E208</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/thrustProtection</v>
       </c>
-    </row>
-    <row r="209" spans="1:8">
+      <c r="I208" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9">
       <c r="A209" t="s">
         <v>630</v>
       </c>
@@ -12015,8 +12675,11 @@
         <f>VLOOKUP(A209,Overview!B:D,3,0)&amp; "/" &amp; E209</f>
         <v>https://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterExhaustPoint</v>
       </c>
-    </row>
-    <row r="210" spans="1:8">
+      <c r="I209" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9">
       <c r="A210" t="s">
         <v>397</v>
       </c>
@@ -12043,8 +12706,11 @@
         <f>VLOOKUP(A210,Overview!B:D,3,0)&amp; "/" &amp; E210</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsAppurtenanceTypeIMKLValue/splitter</v>
       </c>
-    </row>
-    <row r="211" spans="1:8">
+      <c r="I210" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9">
       <c r="A211" t="s">
         <v>397</v>
       </c>
@@ -12071,8 +12737,11 @@
         <f>VLOOKUP(A211,Overview!B:D,3,0)&amp; "/" &amp; E211</f>
         <v>https://vocab.belgif.be/auth/IMKL-TelecommunicationsAppurtenanceTypeIMKLValue/termination</v>
       </c>
-    </row>
-    <row r="212" spans="1:8">
+      <c r="I211" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9">
       <c r="A212" t="s">
         <v>634</v>
       </c>
@@ -12096,8 +12765,11 @@
         <f>VLOOKUP(A212,Overview!B:D,3,0)&amp; "/" &amp; E212</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/electricity</v>
       </c>
-    </row>
-    <row r="213" spans="1:8">
+      <c r="I212" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9">
       <c r="A213" t="s">
         <v>634</v>
       </c>
@@ -12121,8 +12793,11 @@
         <f>VLOOKUP(A213,Overview!B:D,3,0)&amp; "/" &amp; E213</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/oilGasChemical</v>
       </c>
-    </row>
-    <row r="214" spans="1:8">
+      <c r="I213" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9">
       <c r="A214" t="s">
         <v>634</v>
       </c>
@@ -12146,8 +12821,11 @@
         <f>VLOOKUP(A214,Overview!B:D,3,0)&amp; "/" &amp; E214</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/sewer</v>
       </c>
-    </row>
-    <row r="215" spans="1:8">
+      <c r="I214" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9">
       <c r="A215" t="s">
         <v>634</v>
       </c>
@@ -12171,8 +12849,11 @@
         <f>VLOOKUP(A215,Overview!B:D,3,0)&amp; "/" &amp; E215</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/telecommunications</v>
       </c>
-    </row>
-    <row r="216" spans="1:8">
+      <c r="I215" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9">
       <c r="A216" t="s">
         <v>634</v>
       </c>
@@ -12196,8 +12877,11 @@
         <f>VLOOKUP(A216,Overview!B:D,3,0)&amp; "/" &amp; E216</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/thermal</v>
       </c>
-    </row>
-    <row r="217" spans="1:8">
+      <c r="I216" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9">
       <c r="A217" t="s">
         <v>634</v>
       </c>
@@ -12221,8 +12905,11 @@
         <f>VLOOKUP(A217,Overview!B:D,3,0)&amp; "/" &amp; E217</f>
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/water</v>
       </c>
-    </row>
-    <row r="218" spans="1:8">
+      <c r="I217" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9">
       <c r="A218" t="s">
         <v>653</v>
       </c>
@@ -12249,8 +12936,11 @@
         <f>VLOOKUP(A218,Overview!B:D,3,0)&amp; "/" &amp; E218</f>
         <v>https://vocab.belgif.be/auth/IMKL-UtilityNetworkTypeIMKLValue/crossTheme</v>
       </c>
-    </row>
-    <row r="219" spans="1:8">
+      <c r="I218" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9">
       <c r="A219" t="s">
         <v>403</v>
       </c>
@@ -12277,8 +12967,11 @@
         <f>VLOOKUP(A219,Overview!B:D,3,0)&amp; "/" &amp; E219</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalProductTypeIMKLValue/coolingWater</v>
       </c>
-    </row>
-    <row r="220" spans="1:8">
+      <c r="I219" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9">
       <c r="A220" t="s">
         <v>403</v>
       </c>
@@ -12305,8 +12998,11 @@
         <f>VLOOKUP(A220,Overview!B:D,3,0)&amp; "/" &amp; E220</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalProductTypeIMKLValue/heatingSteam</v>
       </c>
-    </row>
-    <row r="221" spans="1:8">
+      <c r="I220" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9">
       <c r="A221" t="s">
         <v>403</v>
       </c>
@@ -12333,8 +13029,11 @@
         <f>VLOOKUP(A221,Overview!B:D,3,0)&amp; "/" &amp; E221</f>
         <v>https://vocab.belgif.be/auth/IMKL-ThermalProductTypeIMKLValue/heatingWater</v>
       </c>
-    </row>
-    <row r="222" spans="1:8">
+      <c r="I221" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -12358,8 +13057,11 @@
         <f>VLOOKUP(A222,Overview!B:D,3,0)&amp; "/" &amp; E222</f>
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
-    </row>
-    <row r="223" spans="1:8">
+      <c r="I222" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9">
       <c r="A223" t="s">
         <v>8</v>
       </c>
@@ -12383,8 +13085,11 @@
         <f>VLOOKUP(A223,Overview!B:D,3,0)&amp; "/" &amp; E223</f>
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
-    </row>
-    <row r="224" spans="1:8">
+      <c r="I223" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -12408,8 +13113,11 @@
         <f>VLOOKUP(A224,Overview!B:D,3,0)&amp; "/" &amp; E224</f>
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
-    </row>
-    <row r="225" spans="1:8">
+      <c r="I224" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -12424,8 +13132,11 @@
         <f>VLOOKUP(A225,Overview!B:D,3,0)&amp; "/" &amp; E225</f>
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/underConstruction</v>
       </c>
-    </row>
-    <row r="226" spans="1:8">
+      <c r="I225" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9">
       <c r="A226" t="s">
         <v>516</v>
       </c>
@@ -12449,8 +13160,11 @@
         <f>VLOOKUP(A226,Overview!B:D,3,0)&amp; "/" &amp; E226</f>
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/onGroundSurface</v>
       </c>
-    </row>
-    <row r="227" spans="1:8">
+      <c r="I226" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9">
       <c r="A227" t="s">
         <v>516</v>
       </c>
@@ -12474,8 +13188,11 @@
         <f>VLOOKUP(A227,Overview!B:D,3,0)&amp; "/" &amp; E227</f>
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/suspendedOrElevated</v>
       </c>
-    </row>
-    <row r="228" spans="1:8">
+      <c r="I227" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9">
       <c r="A228" t="s">
         <v>516</v>
       </c>
@@ -12499,8 +13216,11 @@
         <f>VLOOKUP(A228,Overview!B:D,3,0)&amp; "/" &amp; E228</f>
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/underground</v>
       </c>
-    </row>
-    <row r="229" spans="1:8">
+      <c r="I228" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -12517,8 +13237,11 @@
       <c r="H229" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="230" spans="1:8">
+      <c r="I229" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -12535,8 +13258,11 @@
       <c r="H230" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="231" spans="1:8">
+      <c r="I230" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -12553,8 +13279,11 @@
       <c r="H231" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="232" spans="1:8">
+      <c r="I231" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -12571,8 +13300,11 @@
       <c r="H232" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="233" spans="1:8">
+      <c r="I232" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -12589,8 +13321,11 @@
       <c r="H233" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="234" spans="1:8">
+      <c r="I233" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9">
       <c r="A234" t="s">
         <v>18</v>
       </c>
@@ -12614,8 +13349,11 @@
         <f>VLOOKUP(A234,Overview!B:D,3,0)&amp; "/" &amp; E234</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/digitizedPlan</v>
       </c>
-    </row>
-    <row r="235" spans="1:8">
+      <c r="I234" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9">
       <c r="A235" t="s">
         <v>18</v>
       </c>
@@ -12639,8 +13377,11 @@
         <f>VLOOKUP(A235,Overview!B:D,3,0)&amp; "/" &amp; E235</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/gnss</v>
       </c>
-    </row>
-    <row r="236" spans="1:8">
+      <c r="I235" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9">
       <c r="A236" t="s">
         <v>18</v>
       </c>
@@ -12664,8 +13405,11 @@
         <f>VLOOKUP(A236,Overview!B:D,3,0)&amp; "/" &amp; E236</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/lidar</v>
       </c>
-    </row>
-    <row r="237" spans="1:8">
+      <c r="I236" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9">
       <c r="A237" t="s">
         <v>18</v>
       </c>
@@ -12689,8 +13433,11 @@
         <f>VLOOKUP(A237,Overview!B:D,3,0)&amp; "/" &amp; E237</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/measuringTape</v>
       </c>
-    </row>
-    <row r="238" spans="1:8">
+      <c r="I237" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9">
       <c r="A238" t="s">
         <v>18</v>
       </c>
@@ -12714,8 +13461,11 @@
         <f>VLOOKUP(A238,Overview!B:D,3,0)&amp; "/" &amp; E238</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/measuringWheel</v>
       </c>
-    </row>
-    <row r="239" spans="1:8">
+      <c r="I238" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9">
       <c r="A239" t="s">
         <v>18</v>
       </c>
@@ -12739,8 +13489,11 @@
         <f>VLOOKUP(A239,Overview!B:D,3,0)&amp; "/" &amp; E239</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/photogrammetry</v>
       </c>
-    </row>
-    <row r="240" spans="1:8">
+      <c r="I239" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9">
       <c r="A240" t="s">
         <v>18</v>
       </c>
@@ -12764,8 +13517,11 @@
         <f>VLOOKUP(A240,Overview!B:D,3,0)&amp; "/" &amp; E240</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/sketch</v>
       </c>
-    </row>
-    <row r="241" spans="1:8">
+      <c r="I240" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9">
       <c r="A241" t="s">
         <v>18</v>
       </c>
@@ -12789,8 +13545,11 @@
         <f>VLOOKUP(A241,Overview!B:D,3,0)&amp; "/" &amp; E241</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/terrestrial</v>
       </c>
-    </row>
-    <row r="242" spans="1:8">
+      <c r="I241" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9">
       <c r="A242" t="s">
         <v>18</v>
       </c>
@@ -12814,8 +13573,11 @@
         <f>VLOOKUP(A242,Overview!B:D,3,0)&amp; "/" &amp; E242</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/totalStation</v>
       </c>
-    </row>
-    <row r="243" spans="1:8">
+      <c r="I242" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9">
       <c r="A243" t="s">
         <v>18</v>
       </c>
@@ -12839,8 +13601,11 @@
         <f>VLOOKUP(A243,Overview!B:D,3,0)&amp; "/" &amp; E243</f>
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/triangulation</v>
       </c>
-    </row>
-    <row r="244" spans="1:8">
+      <c r="I243" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -12864,8 +13629,11 @@
         <f>VLOOKUP(A244,Overview!B:D,3,0)&amp; "/" &amp; E244</f>
         <v>https://vocab.belgif.be/auth/IMKL-VisibilityTypeValue/notVisibleAboveGround</v>
       </c>
-    </row>
-    <row r="245" spans="1:8">
+      <c r="I244" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9">
       <c r="A245" t="s">
         <v>13</v>
       </c>
@@ -12889,8 +13657,11 @@
         <f>VLOOKUP(A245,Overview!B:D,3,0)&amp; "/" &amp; E245</f>
         <v>https://vocab.belgif.be/auth/IMKL-VisibilityTypeValue/visibleAboveGround</v>
       </c>
-    </row>
-    <row r="246" spans="1:8">
+      <c r="I245" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9">
       <c r="A246" t="s">
         <v>17</v>
       </c>
@@ -12914,8 +13685,11 @@
         <f>VLOOKUP(A246,Overview!B:D,3,0)&amp; "/" &amp; E246</f>
         <v>https://vocab.belgif.be/auth/IMKL-ReferenceSurfaceTypeValue/surfaceLevel</v>
       </c>
-    </row>
-    <row r="247" spans="1:8">
+      <c r="I246" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9">
       <c r="A247" t="s">
         <v>552</v>
       </c>
@@ -12939,8 +13713,11 @@
         <f>VLOOKUP(A247,Overview!B:D,3,0)&amp; "/" &amp; E247</f>
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/culvert</v>
       </c>
-    </row>
-    <row r="248" spans="1:8">
+      <c r="I247" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9">
       <c r="A248" t="s">
         <v>552</v>
       </c>
@@ -12964,8 +13741,11 @@
         <f>VLOOKUP(A248,Overview!B:D,3,0)&amp; "/" &amp; E248</f>
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/directionalDrilling</v>
       </c>
-    </row>
-    <row r="249" spans="1:8">
+      <c r="I248" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9">
       <c r="A249" t="s">
         <v>552</v>
       </c>
@@ -12989,8 +13769,11 @@
         <f>VLOOKUP(A249,Overview!B:D,3,0)&amp; "/" &amp; E249</f>
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/openTrench</v>
       </c>
-    </row>
-    <row r="250" spans="1:8">
+      <c r="I249" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9">
       <c r="A250" t="s">
         <v>552</v>
       </c>
@@ -13014,13 +13797,12 @@
         <f>VLOOKUP(A250,Overview!B:D,3,0)&amp; "/" &amp; E250</f>
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/other</v>
       </c>
+      <c r="I250" t="s">
+        <v>850</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A176:H179">
-      <sortCondition ref="E1:E250"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Replace type with referenceSurfaceType and remove elevatedRisk
</commit_message>
<xml_diff>
--- a/implementation/IMKL3_Codelists.xlsx
+++ b/implementation/IMKL3_Codelists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\IMKL 3\Implementatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E145F50-ECA0-4E97-879C-01E7B8D7ADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA04D52-903B-42FF-BF46-D294E7FA98CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -2519,9 +2519,6 @@
     <t>Twisted pair.</t>
   </si>
   <si>
-    <t>E.g. cables used to transport data.</t>
-  </si>
-  <si>
     <t>Cabling for local distribution of radio, TV, data and telephone signals up to the user's connection point(s).</t>
   </si>
   <si>
@@ -2632,6 +2629,9 @@
   </si>
   <si>
     <t>isobutane</t>
+  </si>
+  <si>
+    <t>E.g. cables used to convey data.</t>
   </si>
 </sst>
 </file>
@@ -3094,37 +3094,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12F05A2-F84B-4BFA-ADF4-7302F1870D77}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="76.7109375" customWidth="1"/>
-    <col min="5" max="5" width="81.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" customWidth="1"/>
+    <col min="5" max="5" width="81.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3979,14 +3979,14 @@
   <dimension ref="A1:D155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6333,20 +6333,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="75.85546875" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="53.28515625" customWidth="1"/>
-    <col min="8" max="8" width="97.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="75.88671875" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="53.33203125" customWidth="1"/>
+    <col min="8" max="8" width="97.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -6354,7 +6354,7 @@
         <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>533</v>
@@ -6375,7 +6375,7 @@
         <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6644,7 +6644,7 @@
         <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>822</v>
+        <v>858</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>559</v>
@@ -6675,7 +6675,7 @@
         <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>559</v>
@@ -6706,7 +6706,7 @@
         <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>559</v>
@@ -6747,7 +6747,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasDistributionLowPressure</v>
       </c>
       <c r="I13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -6778,7 +6778,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasDistributionMediumPressure</v>
       </c>
       <c r="I14" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -6809,7 +6809,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/naturalGasTransport</v>
       </c>
       <c r="I15" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6840,10 +6840,10 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsSubthemeValue/oilGasChemicalsTransport</v>
       </c>
       <c r="I16" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="60">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.2">
       <c r="A17" t="s">
         <v>529</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>559</v>
@@ -6874,7 +6874,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="195">
+    <row r="18" spans="1:9" ht="172.8">
       <c r="A18" t="s">
         <v>529</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>94</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>559</v>
@@ -7109,7 +7109,7 @@
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>559</v>
@@ -7140,7 +7140,7 @@
         <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>559</v>
@@ -7171,7 +7171,7 @@
         <v>129</v>
       </c>
       <c r="F27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>559</v>
@@ -7202,7 +7202,7 @@
         <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>559</v>
@@ -7243,7 +7243,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/drinkingWaterExtractionArea</v>
       </c>
       <c r="I29" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -7302,7 +7302,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/infiltrationArea</v>
       </c>
       <c r="I31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -7333,7 +7333,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/otherProtectedArea</v>
       </c>
       <c r="I32" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -7364,7 +7364,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ProtectedAreaTypeValue/undergroundGasStorage</v>
       </c>
       <c r="I33" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -7395,7 +7395,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/annotationLabel</v>
       </c>
       <c r="I34" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -7426,7 +7426,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/annotationLine</v>
       </c>
       <c r="I35" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -7457,7 +7457,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/arrow</v>
       </c>
       <c r="I36" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -7488,7 +7488,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningGuideline</v>
       </c>
       <c r="I37" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -7519,7 +7519,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningLabel</v>
       </c>
       <c r="I38" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -7550,7 +7550,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-AnnotationTypeValue/dimensioningLine</v>
       </c>
       <c r="I39" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -7581,7 +7581,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/crossSection</v>
       </c>
       <c r="I40" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -7612,7 +7612,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/detailedPlan</v>
       </c>
       <c r="I41" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -7643,7 +7643,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/directionalDrilling</v>
       </c>
       <c r="I42" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -7674,7 +7674,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/longitudinalSection</v>
       </c>
       <c r="I43" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -7705,7 +7705,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/other</v>
       </c>
       <c r="I44" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -7733,7 +7733,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentTypeValue/precaution</v>
       </c>
       <c r="I45" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -7764,7 +7764,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/JPEG</v>
       </c>
       <c r="I46" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -7795,7 +7795,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/PDF</v>
       </c>
       <c r="I47" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -7826,7 +7826,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/PNG</v>
       </c>
       <c r="I48" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -7857,7 +7857,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-DocumentMediaTypeValue/TIFF</v>
       </c>
       <c r="I49" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -7888,7 +7888,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ContainerTypeValue/cableAndPipeGutter</v>
       </c>
       <c r="I50" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -7919,7 +7919,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ContainerTypeValue/jacketPipe</v>
       </c>
       <c r="I51" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -7950,7 +7950,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/accetone</v>
       </c>
       <c r="I52" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -7981,7 +7981,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/air</v>
       </c>
       <c r="I53" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -8012,7 +8012,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/argon</v>
       </c>
       <c r="I54" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -8043,7 +8043,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/bioGas</v>
       </c>
       <c r="I55" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -8074,7 +8074,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butadiene1,2</v>
       </c>
       <c r="I56" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -8105,7 +8105,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butadiene1,3</v>
       </c>
       <c r="I57" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -8123,7 +8123,7 @@
         <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F58" t="s">
         <v>760</v>
@@ -8136,7 +8136,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/butane</v>
       </c>
       <c r="I58" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -8164,7 +8164,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/carbonDioxide</v>
       </c>
       <c r="I59" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -8182,7 +8182,7 @@
         <v>219</v>
       </c>
       <c r="E60" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F60" t="s">
         <v>762</v>
@@ -8195,7 +8195,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/carbonMonoxide</v>
       </c>
       <c r="I60" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -8213,7 +8213,7 @@
         <v>221</v>
       </c>
       <c r="E61" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F61" t="s">
         <v>752</v>
@@ -8226,7 +8226,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/chlorine</v>
       </c>
       <c r="I61" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -8257,7 +8257,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/concrete</v>
       </c>
       <c r="I62" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -8288,7 +8288,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/crude</v>
       </c>
       <c r="I63" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -8306,7 +8306,7 @@
         <v>227</v>
       </c>
       <c r="E64" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F64" t="s">
         <v>763</v>
@@ -8319,7 +8319,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/dichloroethane</v>
       </c>
       <c r="I64" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -8350,7 +8350,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/diesel</v>
       </c>
       <c r="I65" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -8381,7 +8381,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/empty</v>
       </c>
       <c r="I66" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -8399,7 +8399,7 @@
         <v>230</v>
       </c>
       <c r="E67" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F67" t="s">
         <v>764</v>
@@ -8412,7 +8412,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/ethylene</v>
       </c>
       <c r="I67" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -8443,7 +8443,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasFabricationOfCocs</v>
       </c>
       <c r="I68" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -8474,7 +8474,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasHFx</v>
       </c>
       <c r="I69" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -8505,7 +8505,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/gasoil</v>
       </c>
       <c r="I70" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -8536,7 +8536,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/hydrogen</v>
       </c>
       <c r="I71" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -8554,7 +8554,7 @@
         <v>240</v>
       </c>
       <c r="E72" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F72" t="s">
         <v>767</v>
@@ -8567,7 +8567,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/isobutane</v>
       </c>
       <c r="I72" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -8598,7 +8598,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/JET-A1</v>
       </c>
       <c r="I73" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -8629,7 +8629,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/kerosene</v>
       </c>
       <c r="I74" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -8660,7 +8660,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/liquidAmmonia</v>
       </c>
       <c r="I75" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -8678,7 +8678,7 @@
         <v>248</v>
       </c>
       <c r="E76" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F76" s="13" t="s">
         <v>771</v>
@@ -8691,7 +8691,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/liquidHydrocarbon</v>
       </c>
       <c r="I76" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -8722,7 +8722,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/multiProduct</v>
       </c>
       <c r="I77" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -8753,7 +8753,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/MVC</v>
       </c>
       <c r="I78" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -8784,7 +8784,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/naturalGas</v>
       </c>
       <c r="I79" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -8815,7 +8815,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/nitrogen</v>
       </c>
       <c r="I80" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -8846,7 +8846,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/oxygen</v>
       </c>
       <c r="I81" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -8877,7 +8877,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/phenol</v>
       </c>
       <c r="I82" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -8908,7 +8908,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/propane</v>
       </c>
       <c r="I83" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -8939,7 +8939,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/propylene</v>
       </c>
       <c r="I84" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -8970,7 +8970,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/saltWater</v>
       </c>
       <c r="I85" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -9001,7 +9001,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/sand</v>
       </c>
       <c r="I86" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -9032,7 +9032,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/saumur</v>
       </c>
       <c r="I87" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -9063,7 +9063,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/tetrachloroide</v>
       </c>
       <c r="I88" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -9094,7 +9094,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/unknown</v>
       </c>
       <c r="I89" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -9125,7 +9125,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsProductTypeIMKLValue/water</v>
       </c>
       <c r="I90" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -9249,7 +9249,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/adapter</v>
       </c>
       <c r="I94" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -9280,7 +9280,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/airBeacon</v>
       </c>
       <c r="I95" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -9311,7 +9311,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/blowHole</v>
       </c>
       <c r="I96" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -9342,7 +9342,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionInstallation</v>
       </c>
       <c r="I97" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -9373,7 +9373,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/cathodicProtectionMeasurementPoint</v>
       </c>
       <c r="I98" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -9404,7 +9404,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/endCap</v>
       </c>
       <c r="I99" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -9435,7 +9435,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/flange</v>
       </c>
       <c r="I100" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -9466,7 +9466,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/measurementPoint</v>
       </c>
       <c r="I101" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -9497,7 +9497,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/siphon</v>
       </c>
       <c r="I102" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -9528,7 +9528,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/sleeve</v>
       </c>
       <c r="I103" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -9559,7 +9559,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/sluice</v>
       </c>
       <c r="I104" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -9590,7 +9590,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/stoppleFitting</v>
       </c>
       <c r="I105" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -9621,7 +9621,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-OilGasChemicalsAppurtenanceTypeIMKLValue/valve</v>
       </c>
       <c r="I106" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -9974,7 +9974,7 @@
         <v>330</v>
       </c>
       <c r="F118" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G118" s="8" t="s">
         <v>559</v>
@@ -10033,7 +10033,7 @@
         <v>618</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>531</v>
@@ -10099,7 +10099,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/concretePaving</v>
       </c>
       <c r="I122" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -10117,7 +10117,7 @@
         <v>556</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G123" s="9" t="s">
         <v>531</v>
@@ -10127,7 +10127,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-WarningTypeIMKLValue/geotextile</v>
       </c>
       <c r="I123" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -10179,7 +10179,7 @@
         <v>341</v>
       </c>
       <c r="F125" s="13" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G125" s="8" t="s">
         <v>559</v>
@@ -10303,7 +10303,7 @@
         <v>343</v>
       </c>
       <c r="F129" s="13" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G129" s="8" t="s">
         <v>559</v>
@@ -10365,7 +10365,7 @@
         <v>339</v>
       </c>
       <c r="F131" s="13" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G131" s="8" t="s">
         <v>559</v>
@@ -10421,7 +10421,7 @@
         <v>621</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G133" s="9" t="s">
         <v>531</v>
@@ -10446,7 +10446,7 @@
         <v>620</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G134" s="9" t="s">
         <v>531</v>
@@ -10642,7 +10642,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/brickwork</v>
       </c>
       <c r="I140" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -10673,7 +10673,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/concrete</v>
       </c>
       <c r="I141" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -10704,7 +10704,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/crossLinkPolyethylene</v>
       </c>
       <c r="I142" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -10735,7 +10735,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/ductileCastIron</v>
       </c>
       <c r="I143" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -10766,7 +10766,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/ductileCastIronBlutop</v>
       </c>
       <c r="I144" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -10797,7 +10797,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/fiberCement</v>
       </c>
       <c r="I145" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -10828,7 +10828,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/galvanisedSteel</v>
       </c>
       <c r="I146" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -10859,7 +10859,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/glassFiberReinforcedPolyester</v>
       </c>
       <c r="I147" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -10890,7 +10890,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/grayCastIron</v>
       </c>
       <c r="I148" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -10921,7 +10921,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/jute</v>
       </c>
       <c r="I149" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -10952,7 +10952,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/lead</v>
       </c>
       <c r="I150" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -10983,7 +10983,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/other</v>
       </c>
       <c r="I151" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -11014,7 +11014,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethylene</v>
       </c>
       <c r="I152" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -11045,7 +11045,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethyleneHighDensity</v>
       </c>
       <c r="I153" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -11076,7 +11076,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polyethyleneSafetyLine</v>
       </c>
       <c r="I154" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -11107,7 +11107,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polypropylene</v>
       </c>
       <c r="I155" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -11138,7 +11138,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/polypropyleneSLA</v>
       </c>
       <c r="I156" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -11169,7 +11169,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/prestressedConcrete</v>
       </c>
       <c r="I157" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -11200,7 +11200,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/pvc</v>
       </c>
       <c r="I158" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -11231,7 +11231,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/sideroCement</v>
       </c>
       <c r="I159" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -11262,7 +11262,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/stainlessSteel</v>
       </c>
       <c r="I160" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -11293,7 +11293,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/steel</v>
       </c>
       <c r="I161" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -11324,7 +11324,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/stoneware</v>
       </c>
       <c r="I162" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -11355,7 +11355,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/sulfurConcrete</v>
       </c>
       <c r="I163" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -11386,7 +11386,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-MaterialTypeValue/unknown</v>
       </c>
       <c r="I164" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -11469,7 +11469,7 @@
         <v>406</v>
       </c>
       <c r="F167" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G167" s="8" t="s">
         <v>559</v>
@@ -11855,7 +11855,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/collection</v>
       </c>
       <c r="I180" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -11883,7 +11883,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/distribution</v>
       </c>
       <c r="I181" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -11911,7 +11911,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/private</v>
       </c>
       <c r="I182" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -11939,7 +11939,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/transport</v>
       </c>
       <c r="I183" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -11960,7 +11960,7 @@
         <v>655</v>
       </c>
       <c r="F184" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G184" s="9" t="s">
         <v>531</v>
@@ -11970,10 +11970,10 @@
         <v>https://vocab.belgif.be/auth/IMKL-UtilityDeliveryTypeIMKLValue/connection</v>
       </c>
       <c r="I184" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="30">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="28.8">
       <c r="A185" t="s">
         <v>635</v>
       </c>
@@ -11998,7 +11998,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/net</v>
       </c>
       <c r="I185" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -12019,7 +12019,7 @@
         <v>336</v>
       </c>
       <c r="F186" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G186" s="8" t="s">
         <v>559</v>
@@ -12029,10 +12029,10 @@
         <v>https://vocab.belgif.be/auth/IMKL-WarningTypeIMKLValue/protectivePlate</v>
       </c>
       <c r="I186" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" ht="60">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="43.2">
       <c r="A187" t="s">
         <v>635</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>https://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
       <c r="I187" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -12141,7 +12141,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
       <c r="I190" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -12169,7 +12169,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
       <c r="I191" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -12197,7 +12197,7 @@
         <v>https://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
       <c r="I192" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -12794,7 +12794,7 @@
         <v>https://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/oilGasChemical</v>
       </c>
       <c r="I213" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -12927,7 +12927,7 @@
         <v>504</v>
       </c>
       <c r="F218" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G218" s="5" t="s">
         <v>649</v>
@@ -12937,7 +12937,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-UtilityNetworkTypeIMKLValue/crossTheme</v>
       </c>
       <c r="I218" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -12958,7 +12958,7 @@
         <v>511</v>
       </c>
       <c r="F219" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="G219" s="8" t="s">
         <v>649</v>
@@ -12989,7 +12989,7 @@
         <v>507</v>
       </c>
       <c r="F220" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G220" s="8" t="s">
         <v>649</v>
@@ -13020,7 +13020,7 @@
         <v>509</v>
       </c>
       <c r="F221" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G221" s="8" t="s">
         <v>649</v>
@@ -13058,7 +13058,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
       <c r="I222" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -13086,7 +13086,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
       <c r="I223" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -13114,7 +13114,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
       <c r="I224" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -13133,7 +13133,7 @@
         <v>https://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/underConstruction</v>
       </c>
       <c r="I225" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -13161,7 +13161,7 @@
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/onGroundSurface</v>
       </c>
       <c r="I226" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -13189,7 +13189,7 @@
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/suspendedOrElevated</v>
       </c>
       <c r="I227" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -13217,7 +13217,7 @@
         <v>https://inspire.ec.europa.eu/codelist/VerticalPositionValue/underground</v>
       </c>
       <c r="I228" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -13238,7 +13238,7 @@
         <v>530</v>
       </c>
       <c r="I229" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -13259,7 +13259,7 @@
         <v>530</v>
       </c>
       <c r="I230" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -13280,7 +13280,7 @@
         <v>530</v>
       </c>
       <c r="I231" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -13301,7 +13301,7 @@
         <v>530</v>
       </c>
       <c r="I232" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -13322,7 +13322,7 @@
         <v>530</v>
       </c>
       <c r="I233" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="234" spans="1:9">
@@ -13350,7 +13350,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/digitizedPlan</v>
       </c>
       <c r="I234" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -13378,7 +13378,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/gnss</v>
       </c>
       <c r="I235" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -13406,7 +13406,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/lidar</v>
       </c>
       <c r="I236" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -13434,7 +13434,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/measuringTape</v>
       </c>
       <c r="I237" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -13462,7 +13462,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/measuringWheel</v>
       </c>
       <c r="I238" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -13490,7 +13490,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/photogrammetry</v>
       </c>
       <c r="I239" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -13518,7 +13518,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/sketch</v>
       </c>
       <c r="I240" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -13546,7 +13546,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/terrestrial</v>
       </c>
       <c r="I241" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -13574,7 +13574,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/totalStation</v>
       </c>
       <c r="I242" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="243" spans="1:9">
@@ -13602,7 +13602,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-SurveyMethodValue/triangulation</v>
       </c>
       <c r="I243" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -13620,7 +13620,7 @@
         <v>15</v>
       </c>
       <c r="F244" s="4" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G244" s="9" t="s">
         <v>531</v>
@@ -13630,7 +13630,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-VisibilityTypeValue/notVisibleAboveGround</v>
       </c>
       <c r="I244" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -13648,7 +13648,7 @@
         <v>14</v>
       </c>
       <c r="F245" s="4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G245" s="9" t="s">
         <v>531</v>
@@ -13658,7 +13658,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-VisibilityTypeValue/visibleAboveGround</v>
       </c>
       <c r="I245" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -13686,7 +13686,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ReferenceSurfaceTypeValue/surfaceLevel</v>
       </c>
       <c r="I246" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -13714,7 +13714,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/culvert</v>
       </c>
       <c r="I247" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -13742,7 +13742,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/directionalDrilling</v>
       </c>
       <c r="I248" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -13770,7 +13770,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/openTrench</v>
       </c>
       <c r="I249" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -13798,7 +13798,7 @@
         <v>https://vocab.belgif.be/auth/IMKL-ConstructionTechniqueValue/other</v>
       </c>
       <c r="I250" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>